<commit_message>
+ access also the local db + delete a note tag
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCE9B793-B215-444A-BAC7-E0B1843BE321}"/>
+  <xr:revisionPtr revIDLastSave="566" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{221C983E-89F3-4711-AE6D-C01869084227}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="-12495" windowWidth="16200" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="102">
   <si>
     <t>N</t>
   </si>
@@ -309,9 +309,6 @@
   </si>
   <si>
     <t>Add tag to note for log in user</t>
-  </si>
-  <si>
-    <t>delete tag to note for log in user</t>
   </si>
   <si>
     <t>View all</t>
@@ -408,6 +405,32 @@
   <si>
     <t>Metodele care sunt facute de admini incep cu admin
 Cele normale for fi fara admin</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Before the elements will be deleted the orphanes shall be archived</t>
+  </si>
+  <si>
+    <t>delete tag from note for log in user</t>
+  </si>
+  <si>
+    <t>Remove orphan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The tags shall not be remove if the perent is removed
+</t>
+  </si>
+  <si>
+    <t>Remove orphan not remove</t>
+  </si>
+  <si>
+    <t>Entries form linking table shall be removed</t>
+  </si>
+  <si>
+    <t>If a note is found by user it can be edited by him
+cum poate sa vada un user o notita si cum poate impaca asta cu sharing</t>
   </si>
 </sst>
 </file>
@@ -534,388 +557,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="54">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1237,6 +878,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1276,6 +935,370 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1371,58 +1394,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2AB95F0A-997C-4A60-893A-C402C47724DF}" name="N" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F6E15414-A725-4A88-94CE-0137EFE7B8F6}" name="Categorie" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{EEE22B11-7605-42D0-9695-0D9B47D4122C}" name="S" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{BF71001F-F5F6-4A8F-9314-E52756A5E54C}" name="Actiune" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{BDD7A213-BDAC-48B4-829D-524419C42642}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2AB95F0A-997C-4A60-893A-C402C47724DF}" name="N" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{F6E15414-A725-4A88-94CE-0137EFE7B8F6}" name="Categorie" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{EEE22B11-7605-42D0-9695-0D9B47D4122C}" name="S" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{BF71001F-F5F6-4A8F-9314-E52756A5E54C}" name="Actiune" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{BDD7A213-BDAC-48B4-829D-524419C42642}" name="Column1" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96D400E0-6F3A-4A4F-B7B3-1DDE9DC0092F}" name="Table136" displayName="Table136" ref="A1:F123" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96D400E0-6F3A-4A4F-B7B3-1DDE9DC0092F}" name="Table136" displayName="Table136" ref="A1:F123" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A1:F123" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E123">
     <sortCondition ref="A1:A123"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D7628B32-36E1-4AAD-BCC2-DBE15AE3A288}" name="N" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{92E6ACD6-AC10-432E-B149-97C9B4FF93DB}" name="S" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{46DA51A3-0AFC-4BAD-90AC-BC1D0B4EB350}" name="Subiect" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{0E9011E1-5C6D-4EA0-8863-54B6CD6F951A}" name="Idee" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{040BA331-0196-4FE3-9159-98587F54059B}" name="Detalii" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{6A1A050C-85AA-4B4D-824C-8D2F5BB52A8C}" name="Altele" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{D7628B32-36E1-4AAD-BCC2-DBE15AE3A288}" name="N" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{92E6ACD6-AC10-432E-B149-97C9B4FF93DB}" name="S" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{46DA51A3-0AFC-4BAD-90AC-BC1D0B4EB350}" name="Subiect" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{0E9011E1-5C6D-4EA0-8863-54B6CD6F951A}" name="Idee" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{040BA331-0196-4FE3-9159-98587F54059B}" name="Detalii" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{6A1A050C-85AA-4B4D-824C-8D2F5BB52A8C}" name="Altele" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7AE42CCE-2F3D-4A2D-9A64-D811029D5849}" name="Table1367" displayName="Table1367" ref="A1:G123" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7AE42CCE-2F3D-4A2D-9A64-D811029D5849}" name="Table1367" displayName="Table1367" ref="A1:G123" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A1:G123" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F123">
     <sortCondition ref="A1:A123"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D39497DB-A5B1-405C-ABF9-784FB5093D9E}" name="N" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{552B6E2B-C748-4592-80A6-F06198265568}" name="S" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{CA6589DF-F818-4280-A795-D9B613C17207}" name="Categori" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{A76965F2-410F-483F-A5C7-C28DF80869A7}" name="Subiect" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{77866754-F604-4AFD-B30F-0B9B42069010}" name="Idee" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{007A6C76-1734-4E52-A225-11FD9E282AD5}" name="Detalii" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{27A6BDE0-42B2-453A-B22C-FCBE2C639359}" name="Altele" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{D39497DB-A5B1-405C-ABF9-784FB5093D9E}" name="N" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{552B6E2B-C748-4592-80A6-F06198265568}" name="S" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{CA6589DF-F818-4280-A795-D9B613C17207}" name="Categori" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{A76965F2-410F-483F-A5C7-C28DF80869A7}" name="Subiect" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{77866754-F604-4AFD-B30F-0B9B42069010}" name="Idee" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{007A6C76-1734-4E52-A225-11FD9E282AD5}" name="Detalii" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{27A6BDE0-42B2-453A-B22C-FCBE2C639359}" name="Altele" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F130" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F130" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:F130" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
     <filterColumn colId="1">
       <filters blank="1">
@@ -1435,50 +1458,50 @@
     <sortCondition ref="A1:A130"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{867A761B-88B0-4ABF-B456-C4E8879A3300}" name="S" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{D3CD6840-B70C-43CD-9CAB-43DF78DC5F53}" name="Clasa" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{BDAD06C9-1E35-4E06-9E0A-F8976EF9241F}" name="Actiune" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{10F82FD2-FA3B-4744-9F8E-8BBF8086317C}" name="Lucru" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{90DACBD6-382A-4516-9493-642A496B48A3}" name="Other" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{867A761B-88B0-4ABF-B456-C4E8879A3300}" name="S" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{D3CD6840-B70C-43CD-9CAB-43DF78DC5F53}" name="Clasa" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{BDAD06C9-1E35-4E06-9E0A-F8976EF9241F}" name="Actiune" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{10F82FD2-FA3B-4744-9F8E-8BBF8086317C}" name="Lucru" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{90DACBD6-382A-4516-9493-642A496B48A3}" name="Other" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8BA42F9-DFED-45EA-AC41-6E0B5C9E450B}" name="Table134" displayName="Table134" ref="A1:G64" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8BA42F9-DFED-45EA-AC41-6E0B5C9E450B}" name="Table134" displayName="Table134" ref="A1:G64" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4AC187AE-6AE2-4BEB-B499-A17E030775F3}" name="N" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{26157288-6E0E-4622-B6FF-6D7FCEA74C7F}" name="O" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{E3D3E698-5804-466F-B57A-35EE00DDB50F}" name="S" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{06199DE7-502A-4366-9BE0-434E4102843E}" name="Categorie" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{905CDAB0-DBAC-4C66-84D2-333728828DA0}" name="Todo" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{8AA007C0-EF3A-49CD-9337-10E6C19D0A5A}" name="Done" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{CF3AF89B-CD81-4A43-B444-E6F531918673}" name="Other" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{4AC187AE-6AE2-4BEB-B499-A17E030775F3}" name="N" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{26157288-6E0E-4622-B6FF-6D7FCEA74C7F}" name="O" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{E3D3E698-5804-466F-B57A-35EE00DDB50F}" name="S" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{06199DE7-502A-4366-9BE0-434E4102843E}" name="Categorie" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{905CDAB0-DBAC-4C66-84D2-333728828DA0}" name="Todo" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{8AA007C0-EF3A-49CD-9337-10E6C19D0A5A}" name="Done" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{CF3AF89B-CD81-4A43-B444-E6F531918673}" name="Other" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A1D70E3-5294-4928-A968-C76C79402048}" name="Table1345" displayName="Table1345" ref="A1:G64" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A1D70E3-5294-4928-A968-C76C79402048}" name="Table1345" displayName="Table1345" ref="A1:G64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8EA2D119-3E27-4566-81D1-1306D8CC3651}" name="N" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{65E039F8-B443-4BD3-BD08-BB9C9AB39762}" name="O" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{C722F227-4153-4370-8D0B-BC8BD2702337}" name="S" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{F0C8AA5A-2740-4F1F-B7C4-BEAC7C4B8938}" name="Categorie" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{E40C8687-72DF-46F5-A761-A03AFAA63494}" name="Todo" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{4D62348B-CDB2-403B-B07F-3DAD12C60F4C}" name="Done" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{CEF8DE16-2E80-4774-AB3E-CC177F386B65}" name="Other" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{8EA2D119-3E27-4566-81D1-1306D8CC3651}" name="N" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{65E039F8-B443-4BD3-BD08-BB9C9AB39762}" name="O" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{C722F227-4153-4370-8D0B-BC8BD2702337}" name="S" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F0C8AA5A-2740-4F1F-B7C4-BEAC7C4B8938}" name="Categorie" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E40C8687-72DF-46F5-A761-A03AFAA63494}" name="Todo" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4D62348B-CDB2-403B-B07F-3DAD12C60F4C}" name="Done" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{CEF8DE16-2E80-4774-AB3E-CC177F386B65}" name="Other" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1783,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,7 +1859,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="13"/>
     </row>
@@ -1849,7 +1872,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="13"/>
     </row>
@@ -2272,8 +2295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7FA840-B515-494B-9270-DA5C4EDAADFC}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,19 +2356,21 @@
         <v>52</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>101</v>
+      </c>
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3250,8 +3275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A89F87F-8119-49DC-8C57-CF2AF058D374}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3274,7 +3299,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>59</v>
@@ -3293,13 +3318,13 @@
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="15"/>
@@ -3308,13 +3333,13 @@
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="15"/>
@@ -3323,13 +3348,13 @@
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="14" t="s">
         <v>84</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>85</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="15"/>
@@ -3338,13 +3363,13 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>88</v>
-      </c>
       <c r="E5" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="15"/>
@@ -3353,32 +3378,44 @@
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>90</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>98</v>
+      </c>
       <c r="F7" s="13"/>
       <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="C8" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="15"/>
     </row>
@@ -4329,7 +4366,7 @@
   <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4386,7 +4423,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="11"/>
@@ -4400,7 +4437,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="11"/>
@@ -4414,17 +4451,17 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -4451,7 +4488,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="F7" s="11"/>
     </row>
@@ -4546,7 +4583,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="11"/>
@@ -4562,7 +4599,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="11"/>
@@ -4636,7 +4673,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="11"/>
@@ -4650,7 +4687,7 @@
         <v>41</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="11"/>
@@ -4706,7 +4743,7 @@
         <v>42</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="11"/>
@@ -4720,7 +4757,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="11"/>
@@ -4804,7 +4841,7 @@
         <v>52</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="11"/>
@@ -4818,7 +4855,7 @@
         <v>52</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="11"/>
@@ -4986,7 +5023,7 @@
         <v>34</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="11"/>
@@ -5000,7 +5037,7 @@
         <v>34</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="11"/>
@@ -5014,10 +5051,10 @@
         <v>34</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F46" s="11"/>
     </row>
@@ -5030,10 +5067,10 @@
         <v>34</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F47" s="11"/>
     </row>
@@ -5046,10 +5083,10 @@
         <v>34</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F48" s="11"/>
     </row>
@@ -5062,10 +5099,10 @@
         <v>34</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F49" s="11"/>
     </row>
@@ -5078,7 +5115,7 @@
         <v>34</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="11"/>
@@ -5236,7 +5273,7 @@
         <v>44</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="11"/>
@@ -5250,7 +5287,7 @@
         <v>44</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="11"/>
@@ -5264,7 +5301,7 @@
         <v>44</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="11"/>
@@ -5278,7 +5315,7 @@
         <v>44</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="11"/>
@@ -5292,7 +5329,7 @@
         <v>44</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="11"/>
@@ -5306,7 +5343,7 @@
         <v>44</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="11"/>
@@ -5319,7 +5356,7 @@
         <v>44</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F68" s="11"/>
     </row>
@@ -5486,7 +5523,7 @@
         <v>47</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="11"/>
@@ -5500,7 +5537,7 @@
         <v>47</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="11"/>
@@ -5514,7 +5551,7 @@
         <v>47</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="11"/>
@@ -5528,7 +5565,7 @@
         <v>47</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="11"/>
@@ -5542,7 +5579,7 @@
         <v>47</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="11"/>
@@ -5556,7 +5593,7 @@
         <v>47</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="11"/>
@@ -5570,7 +5607,7 @@
         <v>47</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="11"/>
@@ -5629,7 +5666,7 @@
         <v>27</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F90" s="11"/>
     </row>
@@ -6030,7 +6067,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6147,12 +6184,16 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>

</xml_diff>

<commit_message>
Topic: Creez View all Find by Id
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="566" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{221C983E-89F3-4711-AE6D-C01869084227}"/>
+  <xr:revisionPtr revIDLastSave="625" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8DA7E95-85B8-4556-90BE-180B7B253FCC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Idee" sheetId="8" r:id="rId2"/>
     <sheet name="CodingRoles" sheetId="11" r:id="rId3"/>
     <sheet name="Implement" sheetId="2" r:id="rId4"/>
-    <sheet name="BE_todo" sheetId="4" r:id="rId5"/>
-    <sheet name="FE_todo" sheetId="6" r:id="rId6"/>
+    <sheet name="Learn" sheetId="14" r:id="rId5"/>
+    <sheet name="BE_todo" sheetId="4" r:id="rId6"/>
+    <sheet name="BE_test" sheetId="13" r:id="rId7"/>
+    <sheet name="FE_todo" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -114,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="119">
   <si>
     <t>N</t>
   </si>
@@ -431,6 +433,62 @@
   <si>
     <t>If a note is found by user it can be edited by him
 cum poate sa vada un user o notita si cum poate impaca asta cu sharing</t>
+  </si>
+  <si>
+    <t>Token default</t>
+  </si>
+  <si>
+    <t>add a defaul token for testing</t>
+  </si>
+  <si>
+    <t>Creez un note1 care are tag1 si tag2
+creez un note2 care are tag1 tag2 si tag3</t>
+  </si>
+  <si>
+    <t>Nu ar trebui sa se stearga tagurile daca sterg o notita notita</t>
+  </si>
+  <si>
+    <t>Se sterge notita
+Se vor sterge legaturile
+Nu se sterg tagurile</t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>Then</t>
+  </si>
+  <si>
+    <t>Scop</t>
+  </si>
+  <si>
+    <t>Sterg note1</t>
+  </si>
+  <si>
+    <t>Propagation</t>
+  </si>
+  <si>
+    <t>Sa inteleg mai bine cum se face delete:
+	Cum se face stergerea orfanilor
+Sa verific in ce conditii se face stergeea orfanilor la toate legaturile</t>
+  </si>
+  <si>
+    <t>LogInUser</t>
+  </si>
+  <si>
+    <t>cannot be done somhow static</t>
+  </si>
+  <si>
+    <t>DTO</t>
+  </si>
+  <si>
+    <t>Update all FDTO</t>
+  </si>
+  <si>
+    <t>update all full DTOS</t>
   </si>
 </sst>
 </file>
@@ -512,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -552,11 +610,329 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="74">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1369,10 +1745,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Table Style 1" pivot="0" count="4" xr9:uid="{803E0FE5-88DA-4CC3-8742-6FED218BE0BD}">
-      <tableStyleElement type="wholeTable" dxfId="53"/>
-      <tableStyleElement type="headerRow" dxfId="52"/>
-      <tableStyleElement type="firstRowStripe" dxfId="51"/>
-      <tableStyleElement type="secondRowStripe" dxfId="50"/>
+      <tableStyleElement type="wholeTable" dxfId="73"/>
+      <tableStyleElement type="headerRow" dxfId="72"/>
+      <tableStyleElement type="firstRowStripe" dxfId="71"/>
+      <tableStyleElement type="secondRowStripe" dxfId="70"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1393,59 +1769,63 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2AB95F0A-997C-4A60-893A-C402C47724DF}" name="N" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{F6E15414-A725-4A88-94CE-0137EFE7B8F6}" name="Categorie" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{EEE22B11-7605-42D0-9695-0D9B47D4122C}" name="S" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{BF71001F-F5F6-4A8F-9314-E52756A5E54C}" name="Actiune" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{BDD7A213-BDAC-48B4-829D-524419C42642}" name="Column1" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{2AB95F0A-997C-4A60-893A-C402C47724DF}" name="N" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{F6E15414-A725-4A88-94CE-0137EFE7B8F6}" name="Categorie" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{EEE22B11-7605-42D0-9695-0D9B47D4122C}" name="S" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{BF71001F-F5F6-4A8F-9314-E52756A5E54C}" name="Actiune" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{BDD7A213-BDAC-48B4-829D-524419C42642}" name="Column1" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96D400E0-6F3A-4A4F-B7B3-1DDE9DC0092F}" name="Table136" displayName="Table136" ref="A1:F123" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96D400E0-6F3A-4A4F-B7B3-1DDE9DC0092F}" name="Table136" displayName="Table136" ref="A1:F123" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:F123" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E123">
     <sortCondition ref="A1:A123"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D7628B32-36E1-4AAD-BCC2-DBE15AE3A288}" name="N" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{92E6ACD6-AC10-432E-B149-97C9B4FF93DB}" name="S" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{46DA51A3-0AFC-4BAD-90AC-BC1D0B4EB350}" name="Subiect" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{0E9011E1-5C6D-4EA0-8863-54B6CD6F951A}" name="Idee" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{040BA331-0196-4FE3-9159-98587F54059B}" name="Detalii" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{6A1A050C-85AA-4B4D-824C-8D2F5BB52A8C}" name="Altele" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{D7628B32-36E1-4AAD-BCC2-DBE15AE3A288}" name="N" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{92E6ACD6-AC10-432E-B149-97C9B4FF93DB}" name="S" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{46DA51A3-0AFC-4BAD-90AC-BC1D0B4EB350}" name="Subiect" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{0E9011E1-5C6D-4EA0-8863-54B6CD6F951A}" name="Idee" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{040BA331-0196-4FE3-9159-98587F54059B}" name="Detalii" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{6A1A050C-85AA-4B4D-824C-8D2F5BB52A8C}" name="Altele" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7AE42CCE-2F3D-4A2D-9A64-D811029D5849}" name="Table1367" displayName="Table1367" ref="A1:G123" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7AE42CCE-2F3D-4A2D-9A64-D811029D5849}" name="Table1367" displayName="Table1367" ref="A1:G123" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:G123" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F123">
     <sortCondition ref="A1:A123"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D39497DB-A5B1-405C-ABF9-784FB5093D9E}" name="N" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{552B6E2B-C748-4592-80A6-F06198265568}" name="S" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{CA6589DF-F818-4280-A795-D9B613C17207}" name="Categori" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{A76965F2-410F-483F-A5C7-C28DF80869A7}" name="Subiect" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{77866754-F604-4AFD-B30F-0B9B42069010}" name="Idee" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{007A6C76-1734-4E52-A225-11FD9E282AD5}" name="Detalii" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{27A6BDE0-42B2-453A-B22C-FCBE2C639359}" name="Altele" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{D39497DB-A5B1-405C-ABF9-784FB5093D9E}" name="N" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{552B6E2B-C748-4592-80A6-F06198265568}" name="S" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{CA6589DF-F818-4280-A795-D9B613C17207}" name="Categori" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{A76965F2-410F-483F-A5C7-C28DF80869A7}" name="Subiect" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{77866754-F604-4AFD-B30F-0B9B42069010}" name="Idee" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{007A6C76-1734-4E52-A225-11FD9E282AD5}" name="Detalii" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{27A6BDE0-42B2-453A-B22C-FCBE2C639359}" name="Altele" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F130" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F130" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A1:F130" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
     <filterColumn colId="1">
       <filters blank="1">
@@ -1454,54 +1834,94 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F130">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:F130">
     <sortCondition ref="A1:A130"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{867A761B-88B0-4ABF-B456-C4E8879A3300}" name="S" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{D3CD6840-B70C-43CD-9CAB-43DF78DC5F53}" name="Clasa" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{BDAD06C9-1E35-4E06-9E0A-F8976EF9241F}" name="Actiune" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{10F82FD2-FA3B-4744-9F8E-8BBF8086317C}" name="Lucru" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{90DACBD6-382A-4516-9493-642A496B48A3}" name="Other" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{867A761B-88B0-4ABF-B456-C4E8879A3300}" name="S" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{D3CD6840-B70C-43CD-9CAB-43DF78DC5F53}" name="Clasa" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{BDAD06C9-1E35-4E06-9E0A-F8976EF9241F}" name="Actiune" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{10F82FD2-FA3B-4744-9F8E-8BBF8086317C}" name="Lucru" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{90DACBD6-382A-4516-9493-642A496B48A3}" name="Other" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8BA42F9-DFED-45EA-AC41-6E0B5C9E450B}" name="Table134" displayName="Table134" ref="A1:G64" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B9E3B11C-1970-4BFF-A50E-74D52AF99C97}" name="Table1349" displayName="Table1349" ref="A1:G64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4AC187AE-6AE2-4BEB-B499-A17E030775F3}" name="N" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{26157288-6E0E-4622-B6FF-6D7FCEA74C7F}" name="O" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{E3D3E698-5804-466F-B57A-35EE00DDB50F}" name="S" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{06199DE7-502A-4366-9BE0-434E4102843E}" name="Categorie" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{905CDAB0-DBAC-4C66-84D2-333728828DA0}" name="Todo" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{8AA007C0-EF3A-49CD-9337-10E6C19D0A5A}" name="Done" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{CF3AF89B-CD81-4A43-B444-E6F531918673}" name="Other" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{AAC6E595-E99D-4DB1-90E5-47DC31EECFA8}" name="N" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{001B6DB2-FA88-4CB6-B9E6-565C4EA7654F}" name="O" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{E4011D19-60DB-47C2-966A-2D32DC442A47}" name="S" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{B695BADD-9DBE-47D9-BA56-ED21B92A1828}" name="Categorie" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{3D686112-17E6-42F3-89F6-BC315ABBA6D6}" name="Todo" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{6783A8A6-9E60-465A-8F8C-E3458EA428FD}" name="Done" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{735045F8-2FCE-4A18-99FF-9394759A9FCA}" name="Other" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A1D70E3-5294-4928-A968-C76C79402048}" name="Table1345" displayName="Table1345" ref="A1:G64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8BA42F9-DFED-45EA-AC41-6E0B5C9E450B}" name="Table134" displayName="Table134" ref="A1:G64" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8EA2D119-3E27-4566-81D1-1306D8CC3651}" name="N" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{65E039F8-B443-4BD3-BD08-BB9C9AB39762}" name="O" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{C722F227-4153-4370-8D0B-BC8BD2702337}" name="S" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F0C8AA5A-2740-4F1F-B7C4-BEAC7C4B8938}" name="Categorie" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E40C8687-72DF-46F5-A761-A03AFAA63494}" name="Todo" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4D62348B-CDB2-403B-B07F-3DAD12C60F4C}" name="Done" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{CEF8DE16-2E80-4774-AB3E-CC177F386B65}" name="Other" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4AC187AE-6AE2-4BEB-B499-A17E030775F3}" name="N" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{26157288-6E0E-4622-B6FF-6D7FCEA74C7F}" name="O" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{E3D3E698-5804-466F-B57A-35EE00DDB50F}" name="S" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{06199DE7-502A-4366-9BE0-434E4102843E}" name="Categorie" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{905CDAB0-DBAC-4C66-84D2-333728828DA0}" name="Todo" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{8AA007C0-EF3A-49CD-9337-10E6C19D0A5A}" name="Done" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{CF3AF89B-CD81-4A43-B444-E6F531918673}" name="Other" dataDxfId="29"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C98A4A27-05C0-44E7-9CF2-3E94DCEAB4D7}" name="Table1348" displayName="Table1348" ref="A1:I64" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F64">
+    <sortCondition ref="D1:D64"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{FB6440A4-99DA-4E49-AA03-808FA3189E2D}" name="N" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{31A17B15-80EB-42E1-A5A0-335529E67891}" name="O" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{D7C50E10-7A63-4D98-961E-CEBC519A4F3A}" name="S" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{4929AF3D-E527-44F8-83E4-6AE5FF5BA752}" name="Categorie" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{160D8024-BF24-4D71-A879-3001AEF28DB0}" name="Scop" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{68958FAA-582A-40BC-88E4-DFEFCD085D7D}" name="Given" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{58D080F2-3A38-4170-A080-888A61E6472D}" name="When" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{D820C683-EACB-473E-8174-BDFBE5643443}" name="Then" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{FE5DB5B8-32DD-4A39-8CE0-9093E1EA1F43}" name="Other" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A1D70E3-5294-4928-A968-C76C79402048}" name="Table1345" displayName="Table1345" ref="A1:G64" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
+    <sortCondition ref="D1:D64"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8EA2D119-3E27-4566-81D1-1306D8CC3651}" name="N" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{65E039F8-B443-4BD3-BD08-BB9C9AB39762}" name="O" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{C722F227-4153-4370-8D0B-BC8BD2702337}" name="S" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{F0C8AA5A-2740-4F1F-B7C4-BEAC7C4B8938}" name="Categorie" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{E40C8687-72DF-46F5-A761-A03AFAA63494}" name="Todo" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{4D62348B-CDB2-403B-B07F-3DAD12C60F4C}" name="Done" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{CEF8DE16-2E80-4774-AB3E-CC177F386B65}" name="Other" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2295,7 +2715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7FA840-B515-494B-9270-DA5C4EDAADFC}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -4365,8 +4785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67517046-6F90-48A1-9B4E-378B133164D8}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4474,12 +4894,12 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -4494,55 +4914,55 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -4551,14 +4971,14 @@
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -4567,14 +4987,14 @@
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -4583,14 +5003,14 @@
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -4599,83 +5019,91 @@
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>32</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -4687,63 +5115,63 @@
         <v>41</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="11"/>
@@ -4757,63 +5185,63 @@
         <v>42</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="11"/>
@@ -4827,7 +5255,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="11"/>
@@ -4841,7 +5269,7 @@
         <v>52</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="11"/>
@@ -4855,63 +5283,63 @@
         <v>52</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="11"/>
@@ -4925,7 +5353,7 @@
         <v>34</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="11"/>
@@ -4939,7 +5367,7 @@
         <v>34</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="11"/>
@@ -4953,7 +5381,7 @@
         <v>34</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="11"/>
@@ -4967,7 +5395,7 @@
         <v>34</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="11"/>
@@ -4981,7 +5409,7 @@
         <v>34</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="11"/>
@@ -4995,7 +5423,7 @@
         <v>34</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="11"/>
@@ -5009,7 +5437,7 @@
         <v>34</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="11"/>
@@ -5023,7 +5451,7 @@
         <v>34</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="11"/>
@@ -5037,7 +5465,7 @@
         <v>34</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="11"/>
@@ -5051,11 +5479,9 @@
         <v>34</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E46" s="1"/>
       <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5067,10 +5493,10 @@
         <v>34</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F47" s="11"/>
     </row>
@@ -5083,10 +5509,10 @@
         <v>34</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F48" s="11"/>
     </row>
@@ -5099,10 +5525,10 @@
         <v>34</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F49" s="11"/>
     </row>
@@ -5115,21 +5541,25 @@
         <v>34</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>35</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="11"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>36</v>
-      </c>
-      <c r="C51" t="s">
-        <v>44</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E51" s="1"/>
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5140,7 +5570,7 @@
         <v>44</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" s="11"/>
     </row>
@@ -5152,7 +5582,7 @@
         <v>44</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="F53" s="11"/>
     </row>
@@ -5164,7 +5594,7 @@
         <v>44</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="F54" s="11"/>
     </row>
@@ -5176,7 +5606,7 @@
         <v>44</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" s="11"/>
     </row>
@@ -5184,14 +5614,12 @@
       <c r="A56">
         <v>36</v>
       </c>
-      <c r="B56" s="1"/>
       <c r="C56" t="s">
         <v>44</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="1"/>
+        <v>8</v>
+      </c>
       <c r="F56" s="11"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5203,7 +5631,7 @@
         <v>44</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="11"/>
@@ -5217,7 +5645,7 @@
         <v>44</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="11"/>
@@ -5231,7 +5659,7 @@
         <v>44</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="11"/>
@@ -5245,7 +5673,7 @@
         <v>44</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="11"/>
@@ -5259,7 +5687,7 @@
         <v>44</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="11"/>
@@ -5273,7 +5701,7 @@
         <v>44</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="11"/>
@@ -5287,7 +5715,7 @@
         <v>44</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="11"/>
@@ -5301,7 +5729,7 @@
         <v>44</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="11"/>
@@ -5315,7 +5743,7 @@
         <v>44</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="11"/>
@@ -5329,7 +5757,7 @@
         <v>44</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="11"/>
@@ -5343,7 +5771,7 @@
         <v>44</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="11"/>
@@ -5352,26 +5780,26 @@
       <c r="A68">
         <v>36</v>
       </c>
+      <c r="B68" s="1"/>
       <c r="C68" t="s">
         <v>44</v>
       </c>
       <c r="D68" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="11"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>36</v>
+      </c>
+      <c r="C69" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F68" s="11"/>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>37</v>
-      </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E69" s="1"/>
       <c r="F69" s="11"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5383,7 +5811,7 @@
         <v>47</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="11"/>
@@ -5397,7 +5825,7 @@
         <v>47</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="11"/>
@@ -5411,7 +5839,7 @@
         <v>47</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="11"/>
@@ -5425,7 +5853,7 @@
         <v>47</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="11"/>
@@ -5439,7 +5867,7 @@
         <v>47</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="11"/>
@@ -5453,7 +5881,7 @@
         <v>47</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="11"/>
@@ -5467,7 +5895,7 @@
         <v>47</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="11"/>
@@ -5481,7 +5909,7 @@
         <v>47</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="11"/>
@@ -5495,7 +5923,7 @@
         <v>47</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="11"/>
@@ -5509,7 +5937,7 @@
         <v>47</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="11"/>
@@ -5523,7 +5951,7 @@
         <v>47</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="11"/>
@@ -5537,7 +5965,7 @@
         <v>47</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="11"/>
@@ -5551,7 +5979,7 @@
         <v>47</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="11"/>
@@ -5565,7 +5993,7 @@
         <v>47</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="11"/>
@@ -5579,7 +6007,7 @@
         <v>47</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="11"/>
@@ -5593,7 +6021,7 @@
         <v>47</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="11"/>
@@ -5607,21 +6035,21 @@
         <v>47</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="11"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="11"/>
@@ -5635,7 +6063,7 @@
         <v>4</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="11"/>
@@ -5649,7 +6077,7 @@
         <v>4</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="11"/>
@@ -5663,25 +6091,25 @@
         <v>4</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E90" s="1"/>
       <c r="F90" s="11"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E91" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F91" s="11"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5693,7 +6121,7 @@
         <v>34</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="11"/>
@@ -5707,7 +6135,7 @@
         <v>34</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="11"/>
@@ -5721,21 +6149,21 @@
         <v>34</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="11"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>43</v>
+      <c r="A95" s="1">
+        <v>42</v>
       </c>
       <c r="B95" s="1"/>
-      <c r="C95" t="s">
-        <v>44</v>
+      <c r="C95" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="11"/>
@@ -5749,7 +6177,7 @@
         <v>44</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="11"/>
@@ -5763,7 +6191,7 @@
         <v>44</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="11"/>
@@ -5777,21 +6205,21 @@
         <v>44</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="11"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+      <c r="A99">
+        <v>43</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" t="s">
         <v>44</v>
       </c>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="D99" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="11"/>
@@ -5805,7 +6233,7 @@
         <v>47</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="11"/>
@@ -5819,7 +6247,7 @@
         <v>47</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="11"/>
@@ -5833,16 +6261,22 @@
         <v>47</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="11"/>
     </row>
     <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
+      <c r="A103" s="1">
+        <v>44</v>
+      </c>
       <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
+      <c r="C103" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E103" s="1"/>
       <c r="F103" s="11"/>
     </row>
@@ -6063,11 +6497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE23E348-29D0-4FF8-A4A5-A0998E1F2F1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85EC9C-25A0-450D-AE0A-75CD9BA1329C}">
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6104,57 +6538,43 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="9" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>31</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
@@ -6162,12 +6582,8 @@
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
@@ -6175,25 +6591,17 @@
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>95</v>
-      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
@@ -6711,6 +7119,1422 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE23E348-29D0-4FF8-A4A5-A0998E1F2F1A}">
+  <dimension ref="A1:G64"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="88.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1D129C-EF4C-42C0-8BBF-F86B855B079C}">
+  <dimension ref="A1:I64"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="48.140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+    </row>
+    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+    </row>
+    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED31B81-665B-464C-9D97-28A7755B1692}">
   <dimension ref="A1:G64"/>
   <sheetViews>

</xml_diff>

<commit_message>
Note: Adaug Remainder Sterg Remainder
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="625" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8DA7E95-85B8-4556-90BE-180B7B253FCC}"/>
+  <xr:revisionPtr revIDLastSave="660" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB68CD1-CF0F-4EC9-8479-67396438FF3B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -116,12 +116,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="128">
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>Clasa</t>
+    <t>Categorie</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
   <si>
     <t>Actiune</t>
@@ -130,229 +133,82 @@
     <t>Column1</t>
   </si>
   <si>
+    <t>Useri</t>
+  </si>
+  <si>
+    <t>Useri o sa vada doar continutul creat de ei sau cel la care sunt share-uti</t>
+  </si>
+  <si>
+    <t>Default userul normal poate sa vada doar operatiile care le-a facut el
+Pentru inceput toate API o sa fie pentru userul normal</t>
+  </si>
+  <si>
+    <t>Metodele care sunt facute de admini incep cu admin
+Cele normale for fi fara admin</t>
+  </si>
+  <si>
+    <t>Subiect</t>
+  </si>
+  <si>
+    <t>Idee</t>
+  </si>
+  <si>
+    <t>Detalii</t>
+  </si>
+  <si>
+    <t>Altele</t>
+  </si>
+  <si>
     <t>Note</t>
   </si>
   <si>
-    <t>Creez</t>
-  </si>
-  <si>
-    <t>Sterg</t>
-  </si>
-  <si>
-    <t>Adaug Tag</t>
-  </si>
-  <si>
-    <t>Sterg Tag</t>
-  </si>
-  <si>
-    <t>Adaug Remainder</t>
-  </si>
-  <si>
-    <t>Sterg Remainder</t>
-  </si>
-  <si>
-    <t>Adaug Topic</t>
-  </si>
-  <si>
-    <t>Sterg Topic</t>
-  </si>
-  <si>
-    <t>Modific text</t>
-  </si>
-  <si>
-    <t>Categorie</t>
-  </si>
-  <si>
-    <t>Useri</t>
-  </si>
-  <si>
-    <t>Useri o sa vada doar continutul creat de ei sau cel la care sunt share-uti</t>
+    <t>Ar trebui sa existe doua notite identice?</t>
+  </si>
+  <si>
+    <t>Ar trebui sa fi macar informat de ca mai exista ceva similar cu acelas nume</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>User care sa aiba acces la tot?</t>
   </si>
   <si>
     <t>O sa fie un user admin care sa poata avea acces la toate documentele din toata baza de date</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Adaug user la shareUserList</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>ShareUserList</t>
-  </si>
-  <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Create join table in note</t>
-  </si>
-  <si>
-    <t>Adaug History</t>
-  </si>
-  <si>
-    <t>Arhivez History</t>
-  </si>
-  <si>
-    <t>Cum o sa fac history ca sa adaug</t>
-  </si>
-  <si>
-    <t>Nu as vrea sa sterg un histry dar as vrea sa il mut undeva unde sa nu imi afecteze filtrarea</t>
-  </si>
-  <si>
-    <t>Streg user la shareUserList</t>
-  </si>
-  <si>
-    <t>ar trebui sa poti sa vezi toate elementele care le sheruiesti cu ceilalti useri notite topicuri</t>
-  </si>
-  <si>
-    <t>Adaug Note</t>
-  </si>
-  <si>
-    <t>Sterg Note</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Tasks</t>
-  </si>
-  <si>
-    <t>Before tasks a cercal progress bar</t>
-  </si>
-  <si>
-    <t>Adaug tasklist</t>
-  </si>
-  <si>
-    <t>Sterg tasklist</t>
-  </si>
-  <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>When a eement is aded can have the variant to modifie existing element</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Remainder</t>
-  </si>
-  <si>
-    <t>Modific</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Adaug task</t>
-  </si>
-  <si>
-    <t>Sterg task</t>
-  </si>
-  <si>
-    <t>Tasklist</t>
-  </si>
-  <si>
-    <t>Modific name date snozz</t>
-  </si>
-  <si>
-    <t>Modific text start end status</t>
-  </si>
-  <si>
-    <t>Task and Tasklist</t>
-  </si>
-  <si>
-    <t>add progress</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Adaug rol</t>
-  </si>
-  <si>
-    <t>Sterg rol</t>
-  </si>
-  <si>
-    <t>Ar trebui sa existe doua notite identice?</t>
-  </si>
-  <si>
-    <t>Altele</t>
-  </si>
-  <si>
-    <t>Idee</t>
-  </si>
-  <si>
-    <t>Detalii</t>
-  </si>
-  <si>
-    <t>Subiect</t>
-  </si>
-  <si>
-    <t>Ar trebui sa fi macar informat de ca mai exista ceva similar cu acelas nume</t>
-  </si>
-  <si>
-    <t>Lucru</t>
-  </si>
-  <si>
-    <t>Dau un mesaj ca mai exista o notita cu acelas nume</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Add tag to note for log in user</t>
-  </si>
-  <si>
-    <t>View all</t>
-  </si>
-  <si>
-    <t>Find by Id</t>
-  </si>
-  <si>
-    <t>Find by name</t>
-  </si>
-  <si>
-    <t>Find by tag</t>
-  </si>
-  <si>
-    <t>Find by topic</t>
-  </si>
-  <si>
-    <t>Find by note</t>
-  </si>
-  <si>
-    <t>Find by task</t>
-  </si>
-  <si>
-    <t>Find by tasklist</t>
-  </si>
-  <si>
-    <t>Find by nume</t>
-  </si>
-  <si>
-    <t>Cand sterg o notita ar trebui sa mi se mi se arhiveze tot sai sa mi se mute in arhiva</t>
+    <t>If a note is found by user it can be edited by him
+cum poate sa vada un user o notita si cum poate impaca asta cu sharing</t>
+  </si>
+  <si>
+    <t>Creator si Users</t>
+  </si>
+  <si>
+    <t>Pentru orice exista un creator 
+Orice element poate sa aiba o lista de useri care pot sa modicice acel element
+Creatorul poate sa modific lista de useri</t>
+  </si>
+  <si>
+    <t>Delete topic note</t>
+  </si>
+  <si>
+    <t>Add/Delete note from topic sau topic from note sau ambele?</t>
+  </si>
+  <si>
+    <t>Categori</t>
   </si>
   <si>
     <t>Structure</t>
   </si>
   <si>
+    <t xml:space="preserve">Structure </t>
+  </si>
+  <si>
     <t>Join table will be place in the parent package</t>
   </si>
   <si>
-    <t>Categori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure </t>
+    <t>Mapper
+DTO</t>
   </si>
   <si>
     <t>DTO in DTO</t>
@@ -361,10 +217,6 @@
     <t xml:space="preserve"> - Cand adaug un nou DTO intr-un alt DTO sa nu uit sa adaug si clasa la uses
         - un User @Mapper(componentModel = "spring", uses = {UserRoleDTOMapper.class,UserTagDTOMapper.class})
     - daca nu nu mi afiseaza datele din DTO corect</t>
-  </si>
-  <si>
-    <t>Mapper
-DTO</t>
   </si>
   <si>
     <t>Controller
@@ -380,72 +232,282 @@
 3. convert (return convert note to noteDTO)</t>
   </si>
   <si>
-    <t>Service se va returna doar elementele de baza exemplu Note</t>
-  </si>
-  <si>
     <t>Service</t>
   </si>
   <si>
     <t>Return from Service</t>
   </si>
   <si>
+    <t>Service se va returna doar elementele de baza exemplu NoteService va returana Note</t>
+  </si>
+  <si>
     <t>Controller</t>
   </si>
   <si>
+    <t>Return from Controller</t>
+  </si>
+  <si>
     <t>In Controller se va returna Ce DTO se doreste</t>
   </si>
   <si>
-    <t>Return from Controller</t>
-  </si>
-  <si>
-    <t>User care sa aiba acces la tot?</t>
-  </si>
-  <si>
-    <t>Default userul normal poate sa vada doar operatiile care le-a facut el
-Pentru inceput toate API o sa fie pentru userul normal</t>
-  </si>
-  <si>
-    <t>Metodele care sunt facute de admini incep cu admin
-Cele normale for fi fara admin</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>Before the elements will be deleted the orphanes shall be archived</t>
-  </si>
-  <si>
-    <t>delete tag from note for log in user</t>
-  </si>
-  <si>
-    <t>Remove orphan</t>
+    <t>Remove orphan not remove</t>
   </si>
   <si>
     <t xml:space="preserve">The tags shall not be remove if the perent is removed
 </t>
   </si>
   <si>
-    <t>Remove orphan not remove</t>
+    <t>Remove orphan</t>
   </si>
   <si>
     <t>Entries form linking table shall be removed</t>
   </si>
   <si>
-    <t>If a note is found by user it can be edited by him
-cum poate sa vada un user o notita si cum poate impaca asta cu sharing</t>
+    <t>Clasa</t>
+  </si>
+  <si>
+    <t>Lucru</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Modific text</t>
+  </si>
+  <si>
+    <t>View all</t>
+  </si>
+  <si>
+    <t>Find by Id</t>
+  </si>
+  <si>
+    <t>Find by name</t>
+  </si>
+  <si>
+    <t>Adaug Tag</t>
+  </si>
+  <si>
+    <t>Add tag to note for log in user</t>
+  </si>
+  <si>
+    <t>Sterg Tag</t>
+  </si>
+  <si>
+    <t>delete tag from note for log in user</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Creez</t>
+  </si>
+  <si>
+    <t>Adaug Topic</t>
+  </si>
+  <si>
+    <t>Sterg Topic</t>
+  </si>
+  <si>
+    <t>Adaug Remainder</t>
+  </si>
+  <si>
+    <t>Sterg Remainder</t>
+  </si>
+  <si>
+    <t>Sterg</t>
+  </si>
+  <si>
+    <t>Find by tag</t>
+  </si>
+  <si>
+    <t>Find by topic</t>
+  </si>
+  <si>
+    <t>Dau un mesaj ca mai exista o notita cu acelas nume</t>
+  </si>
+  <si>
+    <t>DTO</t>
+  </si>
+  <si>
+    <t>Update all FDTO</t>
+  </si>
+  <si>
+    <t>update all full DTOS</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Remainder</t>
+  </si>
+  <si>
+    <t>Modific name date snozz</t>
+  </si>
+  <si>
+    <t>Modific</t>
+  </si>
+  <si>
+    <t>Adaug rol</t>
+  </si>
+  <si>
+    <t>Sterg rol</t>
+  </si>
+  <si>
+    <t>Adaug Note</t>
+  </si>
+  <si>
+    <t>Sterg Note</t>
+  </si>
+  <si>
+    <t>Adaug tasklist</t>
+  </si>
+  <si>
+    <t>Sterg tasklist</t>
+  </si>
+  <si>
+    <t>Find by note</t>
+  </si>
+  <si>
+    <t>Find by task</t>
+  </si>
+  <si>
+    <t>Find by tasklist</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Modific text start end status</t>
+  </si>
+  <si>
+    <t>Tasklist</t>
+  </si>
+  <si>
+    <t>Adaug task</t>
+  </si>
+  <si>
+    <t>Sterg task</t>
+  </si>
+  <si>
+    <t>Find by nume</t>
+  </si>
+  <si>
+    <t>Adaug user la shareUserList</t>
+  </si>
+  <si>
+    <t>Streg user la shareUserList</t>
+  </si>
+  <si>
+    <t>Adaug History</t>
+  </si>
+  <si>
+    <t>Arhivez History</t>
+  </si>
+  <si>
+    <t>Cand sterg o notita ar trebui sa mi se mi se arhiveze tot sai sa mi se mute in arhiva</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Propagation</t>
+  </si>
+  <si>
+    <t>Sa inteleg mai bine cum se face delete:
+	Cum se face stergerea orfanilor
+Sa verific in ce conditii se face stergeea orfanilor la toate legaturile</t>
+  </si>
+  <si>
+    <t>Cum sa injectez un DTO intr-un alt DTO eficient  Cem a facut la User- UserRole si Note_topic este diferit</t>
+  </si>
+  <si>
+    <t>ShareUserList</t>
+  </si>
+  <si>
+    <t>Create join table in note</t>
+  </si>
+  <si>
+    <t>ar trebui sa poti sa vezi toate elementele care le sheruiesti cu ceilalti useri notite topicuri</t>
+  </si>
+  <si>
+    <t>Cum o sa fac history ca sa adaug</t>
+  </si>
+  <si>
+    <t>Nu as vrea sa sterg un histry dar as vrea sa il mut undeva unde sa nu imi afecteze filtrarea</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>When a eement is aded can have the variant to modifie existing element</t>
+  </si>
+  <si>
+    <t>Task and Tasklist</t>
+  </si>
+  <si>
+    <t>add progress</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Before the elements will be deleted the orphanes shall be archived</t>
   </si>
   <si>
     <t>Token default</t>
   </si>
   <si>
     <t>add a defaul token for testing</t>
+  </si>
+  <si>
+    <t>LogInUser</t>
+  </si>
+  <si>
+    <t>cannot be done somhow static
+shall be used getLogIn from userService</t>
+  </si>
+  <si>
+    <t>Cech topc befor inserting</t>
+  </si>
+  <si>
+    <t>If the topic allready exist throw error</t>
+  </si>
+  <si>
+    <t>Throw errors</t>
+  </si>
+  <si>
+    <t>verific daca nu cumva incerc sa arunc de 2 ori err ex TopicNote in repository si in service la check</t>
+  </si>
+  <si>
+    <t>Scop</t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>Then</t>
+  </si>
+  <si>
+    <t>Nu ar trebui sa se stearga tagurile daca sterg o notita notita</t>
   </si>
   <si>
     <t>Creez un note1 care are tag1 si tag2
 creez un note2 care are tag1 tag2 si tag3</t>
   </si>
   <si>
-    <t>Nu ar trebui sa se stearga tagurile daca sterg o notita notita</t>
+    <t>Sterg note1</t>
   </si>
   <si>
     <t>Se sterge notita
@@ -453,42 +515,10 @@
 Nu se sterg tagurile</t>
   </si>
   <si>
-    <t>Given</t>
-  </si>
-  <si>
-    <t>When</t>
-  </si>
-  <si>
-    <t>Then</t>
-  </si>
-  <si>
-    <t>Scop</t>
-  </si>
-  <si>
-    <t>Sterg note1</t>
-  </si>
-  <si>
-    <t>Propagation</t>
-  </si>
-  <si>
-    <t>Sa inteleg mai bine cum se face delete:
-	Cum se face stergerea orfanilor
-Sa verific in ce conditii se face stergeea orfanilor la toate legaturile</t>
-  </si>
-  <si>
-    <t>LogInUser</t>
-  </si>
-  <si>
-    <t>cannot be done somhow static</t>
-  </si>
-  <si>
-    <t>DTO</t>
-  </si>
-  <si>
-    <t>Update all FDTO</t>
-  </si>
-  <si>
-    <t>update all full DTOS</t>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Before tasks a cercal progress bar</t>
   </si>
 </sst>
 </file>
@@ -680,7 +710,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -755,36 +784,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -941,6 +940,36 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -989,6 +1018,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1044,7 +1074,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -1176,7 +1206,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="0"/>
+        <color rgb="FFFFFFFF"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -1355,7 +1385,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1769,10 +1799,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
@@ -1850,78 +1876,78 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B9E3B11C-1970-4BFF-A50E-74D52AF99C97}" name="Table1349" displayName="Table1349" ref="A1:G64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B9E3B11C-1970-4BFF-A50E-74D52AF99C97}" name="Table1349" displayName="Table1349" ref="A1:G64" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AAC6E595-E99D-4DB1-90E5-47DC31EECFA8}" name="N" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{001B6DB2-FA88-4CB6-B9E6-565C4EA7654F}" name="O" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{E4011D19-60DB-47C2-966A-2D32DC442A47}" name="S" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{B695BADD-9DBE-47D9-BA56-ED21B92A1828}" name="Categorie" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{3D686112-17E6-42F3-89F6-BC315ABBA6D6}" name="Todo" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{6783A8A6-9E60-465A-8F8C-E3458EA428FD}" name="Done" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{735045F8-2FCE-4A18-99FF-9394759A9FCA}" name="Other" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AAC6E595-E99D-4DB1-90E5-47DC31EECFA8}" name="N" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{001B6DB2-FA88-4CB6-B9E6-565C4EA7654F}" name="O" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{E4011D19-60DB-47C2-966A-2D32DC442A47}" name="S" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B695BADD-9DBE-47D9-BA56-ED21B92A1828}" name="Categorie" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{3D686112-17E6-42F3-89F6-BC315ABBA6D6}" name="Todo" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{6783A8A6-9E60-465A-8F8C-E3458EA428FD}" name="Done" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{735045F8-2FCE-4A18-99FF-9394759A9FCA}" name="Other" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8BA42F9-DFED-45EA-AC41-6E0B5C9E450B}" name="Table134" displayName="Table134" ref="A1:G64" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8BA42F9-DFED-45EA-AC41-6E0B5C9E450B}" name="Table134" displayName="Table134" ref="A1:G64" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4AC187AE-6AE2-4BEB-B499-A17E030775F3}" name="N" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{26157288-6E0E-4622-B6FF-6D7FCEA74C7F}" name="O" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{E3D3E698-5804-466F-B57A-35EE00DDB50F}" name="S" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{06199DE7-502A-4366-9BE0-434E4102843E}" name="Categorie" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{905CDAB0-DBAC-4C66-84D2-333728828DA0}" name="Todo" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{8AA007C0-EF3A-49CD-9337-10E6C19D0A5A}" name="Done" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{CF3AF89B-CD81-4A43-B444-E6F531918673}" name="Other" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{4AC187AE-6AE2-4BEB-B499-A17E030775F3}" name="N" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{26157288-6E0E-4622-B6FF-6D7FCEA74C7F}" name="O" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{E3D3E698-5804-466F-B57A-35EE00DDB50F}" name="S" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{06199DE7-502A-4366-9BE0-434E4102843E}" name="Categorie" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{905CDAB0-DBAC-4C66-84D2-333728828DA0}" name="Todo" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{8AA007C0-EF3A-49CD-9337-10E6C19D0A5A}" name="Done" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{CF3AF89B-CD81-4A43-B444-E6F531918673}" name="Other" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C98A4A27-05C0-44E7-9CF2-3E94DCEAB4D7}" name="Table1348" displayName="Table1348" ref="A1:I64" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C98A4A27-05C0-44E7-9CF2-3E94DCEAB4D7}" name="Table1348" displayName="Table1348" ref="A1:I64" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:I64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FB6440A4-99DA-4E49-AA03-808FA3189E2D}" name="N" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{31A17B15-80EB-42E1-A5A0-335529E67891}" name="O" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{D7C50E10-7A63-4D98-961E-CEBC519A4F3A}" name="S" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{4929AF3D-E527-44F8-83E4-6AE5FF5BA752}" name="Categorie" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{160D8024-BF24-4D71-A879-3001AEF28DB0}" name="Scop" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{68958FAA-582A-40BC-88E4-DFEFCD085D7D}" name="Given" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{58D080F2-3A38-4170-A080-888A61E6472D}" name="When" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{D820C683-EACB-473E-8174-BDFBE5643443}" name="Then" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{FE5DB5B8-32DD-4A39-8CE0-9093E1EA1F43}" name="Other" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{FB6440A4-99DA-4E49-AA03-808FA3189E2D}" name="N" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{31A17B15-80EB-42E1-A5A0-335529E67891}" name="O" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{D7C50E10-7A63-4D98-961E-CEBC519A4F3A}" name="S" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{4929AF3D-E527-44F8-83E4-6AE5FF5BA752}" name="Categorie" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{160D8024-BF24-4D71-A879-3001AEF28DB0}" name="Scop" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{68958FAA-582A-40BC-88E4-DFEFCD085D7D}" name="Given" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{58D080F2-3A38-4170-A080-888A61E6472D}" name="When" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{D820C683-EACB-473E-8174-BDFBE5643443}" name="Then" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{FE5DB5B8-32DD-4A39-8CE0-9093E1EA1F43}" name="Other" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A1D70E3-5294-4928-A968-C76C79402048}" name="Table1345" displayName="Table1345" ref="A1:G64" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A1D70E3-5294-4928-A968-C76C79402048}" name="Table1345" displayName="Table1345" ref="A1:G64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8EA2D119-3E27-4566-81D1-1306D8CC3651}" name="N" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{65E039F8-B443-4BD3-BD08-BB9C9AB39762}" name="O" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{C722F227-4153-4370-8D0B-BC8BD2702337}" name="S" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{F0C8AA5A-2740-4F1F-B7C4-BEAC7C4B8938}" name="Categorie" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{E40C8687-72DF-46F5-A761-A03AFAA63494}" name="Todo" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{4D62348B-CDB2-403B-B07F-3DAD12C60F4C}" name="Done" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{CEF8DE16-2E80-4774-AB3E-CC177F386B65}" name="Other" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{8EA2D119-3E27-4566-81D1-1306D8CC3651}" name="N" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{65E039F8-B443-4BD3-BD08-BB9C9AB39762}" name="O" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{C722F227-4153-4370-8D0B-BC8BD2702337}" name="S" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F0C8AA5A-2740-4F1F-B7C4-BEAC7C4B8938}" name="Categorie" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E40C8687-72DF-46F5-A761-A03AFAA63494}" name="Todo" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4D62348B-CDB2-403B-B07F-3DAD12C60F4C}" name="Done" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{CEF8DE16-2E80-4774-AB3E-CC177F386B65}" name="Other" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2245,54 +2271,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C2" s="13">
         <v>4</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C3" s="13">
         <v>4</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C4" s="13">
         <v>4</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="E4" s="13"/>
     </row>
@@ -2716,7 +2742,7 @@
   <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2725,7 +2751,7 @@
     <col min="2" max="2" width="4.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="10" customWidth="1"/>
     <col min="4" max="4" width="44.85546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="59.28515625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="86.7109375" style="16" customWidth="1"/>
     <col min="6" max="6" width="81.42578125" style="10" customWidth="1"/>
     <col min="7" max="7" width="72.7109375" style="10" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="10"/>
@@ -2736,22 +2762,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2759,13 +2785,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F2" s="15"/>
     </row>
@@ -2773,40 +2799,48 @@
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="14" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
+      <c r="D5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
+      <c r="D6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3695,8 +3729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A89F87F-8119-49DC-8C57-CF2AF058D374}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,7 +3739,7 @@
     <col min="2" max="2" width="4.7109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="10" customWidth="1"/>
     <col min="4" max="4" width="27.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="61.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="61.85546875" style="16" customWidth="1"/>
     <col min="6" max="6" width="81.42578125" style="10" customWidth="1"/>
     <col min="7" max="7" width="72.7109375" style="10" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="10"/>
@@ -3716,35 +3750,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>76</v>
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="15"/>
@@ -3753,13 +3787,13 @@
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="14" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="15"/>
@@ -3768,28 +3802,28 @@
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="14" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>85</v>
+        <v>35</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="15"/>
@@ -3798,13 +3832,13 @@
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>89</v>
+        <v>38</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="15"/>
@@ -3813,13 +3847,13 @@
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="15"/>
@@ -3828,13 +3862,13 @@
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>100</v>
+        <v>42</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="15"/>
@@ -3844,7 +3878,7 @@
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="13"/>
       <c r="G9" s="15"/>
     </row>
@@ -3853,7 +3887,7 @@
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="13"/>
       <c r="G10" s="15"/>
     </row>
@@ -3862,7 +3896,7 @@
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="13"/>
       <c r="G11" s="15"/>
     </row>
@@ -3871,7 +3905,7 @@
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="13"/>
       <c r="G12" s="15"/>
     </row>
@@ -3880,7 +3914,7 @@
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="13"/>
       <c r="G13" s="15"/>
     </row>
@@ -3889,7 +3923,7 @@
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="13"/>
       <c r="G14" s="15"/>
     </row>
@@ -3898,7 +3932,7 @@
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="13"/>
       <c r="G15" s="15"/>
     </row>
@@ -3907,7 +3941,7 @@
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="13"/>
       <c r="G16" s="15"/>
     </row>
@@ -3916,7 +3950,7 @@
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
@@ -3925,7 +3959,7 @@
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="13"/>
       <c r="G18" s="15"/>
     </row>
@@ -3934,7 +3968,7 @@
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="13"/>
       <c r="G19" s="15"/>
     </row>
@@ -3943,7 +3977,7 @@
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
@@ -3952,7 +3986,7 @@
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="13"/>
       <c r="G21" s="15"/>
     </row>
@@ -3961,7 +3995,7 @@
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
@@ -3970,7 +4004,7 @@
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
@@ -3979,7 +4013,7 @@
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="13"/>
       <c r="G24" s="15"/>
     </row>
@@ -3988,7 +4022,7 @@
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
@@ -3997,7 +4031,7 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="13"/>
       <c r="G26" s="15"/>
     </row>
@@ -4006,7 +4040,7 @@
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
@@ -4015,7 +4049,7 @@
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="13"/>
       <c r="G28" s="15"/>
     </row>
@@ -4024,7 +4058,7 @@
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
@@ -4033,7 +4067,7 @@
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
@@ -4042,7 +4076,7 @@
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="13"/>
       <c r="G31" s="15"/>
     </row>
@@ -4051,7 +4085,7 @@
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="13"/>
       <c r="G32" s="15"/>
     </row>
@@ -4060,7 +4094,7 @@
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="13"/>
       <c r="G33" s="15"/>
     </row>
@@ -4069,7 +4103,7 @@
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
+      <c r="E34" s="14"/>
       <c r="F34" s="13"/>
       <c r="G34" s="15"/>
     </row>
@@ -4078,7 +4112,7 @@
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
+      <c r="E35" s="14"/>
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
@@ -4087,7 +4121,7 @@
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="E36" s="14"/>
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
@@ -4096,7 +4130,7 @@
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
+      <c r="E37" s="14"/>
       <c r="F37" s="13"/>
       <c r="G37" s="15"/>
     </row>
@@ -4105,7 +4139,7 @@
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
+      <c r="E38" s="14"/>
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
@@ -4114,7 +4148,7 @@
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
+      <c r="E39" s="14"/>
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
@@ -4123,7 +4157,7 @@
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
+      <c r="E40" s="14"/>
       <c r="F40" s="13"/>
       <c r="G40" s="15"/>
     </row>
@@ -4132,7 +4166,7 @@
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
+      <c r="E41" s="14"/>
       <c r="F41" s="13"/>
       <c r="G41" s="15"/>
     </row>
@@ -4141,7 +4175,7 @@
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
+      <c r="E42" s="14"/>
       <c r="F42" s="13"/>
       <c r="G42" s="15"/>
     </row>
@@ -4150,7 +4184,7 @@
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
+      <c r="E43" s="14"/>
       <c r="F43" s="13"/>
       <c r="G43" s="15"/>
     </row>
@@ -4159,7 +4193,7 @@
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
+      <c r="E44" s="14"/>
       <c r="F44" s="13"/>
       <c r="G44" s="15"/>
     </row>
@@ -4168,7 +4202,7 @@
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
+      <c r="E45" s="14"/>
       <c r="F45" s="13"/>
       <c r="G45" s="15"/>
     </row>
@@ -4177,7 +4211,7 @@
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="E46" s="14"/>
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
@@ -4186,7 +4220,7 @@
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
+      <c r="E47" s="14"/>
       <c r="F47" s="13"/>
       <c r="G47" s="15"/>
     </row>
@@ -4195,7 +4229,7 @@
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
+      <c r="E48" s="14"/>
       <c r="F48" s="13"/>
       <c r="G48" s="15"/>
     </row>
@@ -4204,7 +4238,7 @@
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
+      <c r="E49" s="14"/>
       <c r="F49" s="13"/>
       <c r="G49" s="15"/>
     </row>
@@ -4213,7 +4247,7 @@
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
+      <c r="E50" s="14"/>
       <c r="F50" s="13"/>
       <c r="G50" s="15"/>
     </row>
@@ -4222,7 +4256,7 @@
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
+      <c r="E51" s="14"/>
       <c r="F51" s="13"/>
       <c r="G51" s="15"/>
     </row>
@@ -4231,7 +4265,7 @@
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
+      <c r="E52" s="14"/>
       <c r="F52" s="13"/>
       <c r="G52" s="15"/>
     </row>
@@ -4240,107 +4274,107 @@
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
+      <c r="E53" s="14"/>
       <c r="F53" s="13"/>
       <c r="G53" s="15"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E54" s="13"/>
+      <c r="E54" s="14"/>
       <c r="G54" s="15"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E55" s="13"/>
+      <c r="E55" s="14"/>
       <c r="G55" s="15"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E56" s="13"/>
+      <c r="E56" s="14"/>
       <c r="G56" s="15"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E57" s="13"/>
+      <c r="E57" s="14"/>
       <c r="G57" s="15"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E58" s="13"/>
+      <c r="E58" s="14"/>
       <c r="G58" s="15"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E59" s="13"/>
+      <c r="E59" s="14"/>
       <c r="F59" s="13"/>
       <c r="G59" s="15"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E60" s="13"/>
+      <c r="E60" s="14"/>
       <c r="F60" s="13"/>
       <c r="G60" s="15"/>
     </row>
     <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E61" s="13"/>
+      <c r="E61" s="14"/>
       <c r="F61" s="13"/>
       <c r="G61" s="15"/>
     </row>
     <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E62" s="13"/>
+      <c r="E62" s="14"/>
       <c r="F62" s="13"/>
       <c r="G62" s="15"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E63" s="13"/>
+      <c r="E63" s="14"/>
       <c r="F63" s="13"/>
       <c r="G63" s="15"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E64" s="13"/>
+      <c r="E64" s="14"/>
       <c r="F64" s="13"/>
       <c r="G64" s="15"/>
     </row>
     <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E65" s="13"/>
+      <c r="E65" s="14"/>
       <c r="F65" s="13"/>
       <c r="G65" s="15"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E66" s="13"/>
+      <c r="E66" s="14"/>
       <c r="F66" s="13"/>
       <c r="G66" s="15"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E67" s="13"/>
+      <c r="E67" s="14"/>
       <c r="F67" s="13"/>
       <c r="G67" s="15"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E68" s="13"/>
+      <c r="E68" s="14"/>
       <c r="F68" s="13"/>
       <c r="G68" s="15"/>
     </row>
     <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E69" s="13"/>
+      <c r="E69" s="14"/>
       <c r="F69" s="13"/>
       <c r="G69" s="15"/>
     </row>
     <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E70" s="13"/>
+      <c r="E70" s="14"/>
       <c r="F70" s="13"/>
       <c r="G70" s="15"/>
     </row>
     <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E71" s="13"/>
+      <c r="E71" s="14"/>
       <c r="F71" s="13"/>
       <c r="G71" s="15"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E72" s="13"/>
+      <c r="E72" s="14"/>
       <c r="F72" s="13"/>
       <c r="G72" s="15"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E73" s="13"/>
+      <c r="E73" s="14"/>
       <c r="F73" s="13"/>
       <c r="G73" s="15"/>
     </row>
     <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E74" s="13"/>
+      <c r="E74" s="14"/>
       <c r="G74" s="15"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -4348,7 +4382,7 @@
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
+      <c r="E75" s="14"/>
       <c r="F75" s="13"/>
       <c r="G75" s="15"/>
     </row>
@@ -4357,7 +4391,7 @@
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
+      <c r="E76" s="14"/>
       <c r="F76" s="13"/>
       <c r="G76" s="15"/>
     </row>
@@ -4366,7 +4400,7 @@
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
+      <c r="E77" s="14"/>
       <c r="F77" s="13"/>
       <c r="G77" s="15"/>
     </row>
@@ -4375,7 +4409,7 @@
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
+      <c r="E78" s="14"/>
       <c r="F78" s="13"/>
       <c r="G78" s="15"/>
     </row>
@@ -4384,7 +4418,7 @@
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
+      <c r="E79" s="14"/>
       <c r="F79" s="13"/>
       <c r="G79" s="15"/>
     </row>
@@ -4393,7 +4427,7 @@
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
+      <c r="E80" s="14"/>
       <c r="F80" s="13"/>
       <c r="G80" s="15"/>
     </row>
@@ -4402,7 +4436,7 @@
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
+      <c r="E81" s="14"/>
       <c r="F81" s="13"/>
       <c r="G81" s="15"/>
     </row>
@@ -4411,7 +4445,7 @@
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
+      <c r="E82" s="14"/>
       <c r="F82" s="13"/>
       <c r="G82" s="15"/>
     </row>
@@ -4420,7 +4454,7 @@
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
       <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
+      <c r="E83" s="14"/>
       <c r="F83" s="13"/>
       <c r="G83" s="15"/>
     </row>
@@ -4429,7 +4463,7 @@
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
       <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
+      <c r="E84" s="14"/>
       <c r="F84" s="13"/>
       <c r="G84" s="15"/>
     </row>
@@ -4438,7 +4472,7 @@
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
-      <c r="E85" s="13"/>
+      <c r="E85" s="14"/>
       <c r="F85" s="13"/>
       <c r="G85" s="15"/>
     </row>
@@ -4447,7 +4481,7 @@
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
+      <c r="E86" s="14"/>
       <c r="F86" s="13"/>
       <c r="G86" s="15"/>
     </row>
@@ -4456,7 +4490,7 @@
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
+      <c r="E87" s="14"/>
       <c r="F87" s="13"/>
       <c r="G87" s="15"/>
     </row>
@@ -4465,7 +4499,7 @@
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
       <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
+      <c r="E88" s="14"/>
       <c r="F88" s="13"/>
       <c r="G88" s="15"/>
     </row>
@@ -4474,7 +4508,7 @@
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
       <c r="D89" s="13"/>
-      <c r="E89" s="13"/>
+      <c r="E89" s="14"/>
       <c r="F89" s="13"/>
       <c r="G89" s="15"/>
     </row>
@@ -4483,7 +4517,7 @@
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
       <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
+      <c r="E90" s="14"/>
       <c r="F90" s="13"/>
       <c r="G90" s="15"/>
     </row>
@@ -4492,7 +4526,7 @@
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
       <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
+      <c r="E91" s="14"/>
       <c r="F91" s="13"/>
       <c r="G91" s="15"/>
     </row>
@@ -4501,7 +4535,7 @@
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
       <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
+      <c r="E92" s="14"/>
       <c r="F92" s="13"/>
       <c r="G92" s="15"/>
     </row>
@@ -4510,7 +4544,7 @@
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
+      <c r="E93" s="14"/>
       <c r="F93" s="13"/>
       <c r="G93" s="15"/>
     </row>
@@ -4519,7 +4553,7 @@
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
       <c r="D94" s="13"/>
-      <c r="E94" s="13"/>
+      <c r="E94" s="14"/>
       <c r="F94" s="13"/>
       <c r="G94" s="15"/>
     </row>
@@ -4528,7 +4562,7 @@
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
       <c r="D95" s="13"/>
-      <c r="E95" s="13"/>
+      <c r="E95" s="14"/>
       <c r="F95" s="13"/>
       <c r="G95" s="15"/>
     </row>
@@ -4537,7 +4571,7 @@
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
       <c r="D96" s="13"/>
-      <c r="E96" s="13"/>
+      <c r="E96" s="14"/>
       <c r="F96" s="13"/>
       <c r="G96" s="15"/>
     </row>
@@ -4546,7 +4580,7 @@
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
       <c r="D97" s="13"/>
-      <c r="E97" s="13"/>
+      <c r="E97" s="14"/>
       <c r="F97" s="13"/>
       <c r="G97" s="15"/>
     </row>
@@ -4555,7 +4589,7 @@
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
       <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
+      <c r="E98" s="14"/>
       <c r="F98" s="13"/>
       <c r="G98" s="15"/>
     </row>
@@ -4564,7 +4598,7 @@
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
-      <c r="E99" s="13"/>
+      <c r="E99" s="14"/>
       <c r="F99" s="13"/>
       <c r="G99" s="15"/>
     </row>
@@ -4573,7 +4607,7 @@
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
       <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
+      <c r="E100" s="14"/>
       <c r="F100" s="13"/>
       <c r="G100" s="15"/>
     </row>
@@ -4588,7 +4622,7 @@
       <c r="B103" s="13"/>
       <c r="C103" s="13"/>
       <c r="D103" s="13"/>
-      <c r="E103" s="13"/>
+      <c r="E103" s="14"/>
       <c r="F103" s="13"/>
       <c r="G103" s="15"/>
     </row>
@@ -4597,7 +4631,7 @@
       <c r="B104" s="13"/>
       <c r="C104" s="13"/>
       <c r="D104" s="13"/>
-      <c r="E104" s="13"/>
+      <c r="E104" s="14"/>
       <c r="F104" s="13"/>
       <c r="G104" s="15"/>
     </row>
@@ -4606,7 +4640,7 @@
       <c r="B105" s="13"/>
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
-      <c r="E105" s="13"/>
+      <c r="E105" s="14"/>
       <c r="F105" s="13"/>
       <c r="G105" s="15"/>
     </row>
@@ -4615,7 +4649,7 @@
       <c r="B106" s="13"/>
       <c r="C106" s="13"/>
       <c r="D106" s="13"/>
-      <c r="E106" s="13"/>
+      <c r="E106" s="14"/>
       <c r="F106" s="13"/>
       <c r="G106" s="15"/>
     </row>
@@ -4624,7 +4658,7 @@
       <c r="B107" s="13"/>
       <c r="C107" s="13"/>
       <c r="D107" s="13"/>
-      <c r="E107" s="13"/>
+      <c r="E107" s="14"/>
       <c r="F107" s="13"/>
       <c r="G107" s="15"/>
     </row>
@@ -4633,7 +4667,7 @@
       <c r="B108" s="13"/>
       <c r="C108" s="13"/>
       <c r="D108" s="13"/>
-      <c r="E108" s="13"/>
+      <c r="E108" s="14"/>
       <c r="F108" s="13"/>
       <c r="G108" s="15"/>
     </row>
@@ -4642,7 +4676,7 @@
       <c r="B109" s="13"/>
       <c r="C109" s="13"/>
       <c r="D109" s="13"/>
-      <c r="E109" s="13"/>
+      <c r="E109" s="14"/>
       <c r="F109" s="13"/>
       <c r="G109" s="15"/>
     </row>
@@ -4651,7 +4685,7 @@
       <c r="B110" s="13"/>
       <c r="C110" s="13"/>
       <c r="D110" s="13"/>
-      <c r="E110" s="13"/>
+      <c r="E110" s="14"/>
       <c r="F110" s="13"/>
       <c r="G110" s="15"/>
     </row>
@@ -4660,7 +4694,7 @@
       <c r="B111" s="13"/>
       <c r="C111" s="13"/>
       <c r="D111" s="13"/>
-      <c r="E111" s="13"/>
+      <c r="E111" s="14"/>
       <c r="F111" s="13"/>
       <c r="G111" s="15"/>
     </row>
@@ -4669,7 +4703,7 @@
       <c r="B112" s="13"/>
       <c r="C112" s="13"/>
       <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
+      <c r="E112" s="14"/>
       <c r="F112" s="13"/>
       <c r="G112" s="15"/>
     </row>
@@ -4678,7 +4712,7 @@
       <c r="B113" s="13"/>
       <c r="C113" s="13"/>
       <c r="D113" s="13"/>
-      <c r="E113" s="13"/>
+      <c r="E113" s="14"/>
       <c r="F113" s="13"/>
       <c r="G113" s="15"/>
     </row>
@@ -4687,7 +4721,7 @@
       <c r="B114" s="13"/>
       <c r="C114" s="13"/>
       <c r="D114" s="13"/>
-      <c r="E114" s="13"/>
+      <c r="E114" s="14"/>
       <c r="F114" s="13"/>
       <c r="G114" s="15"/>
     </row>
@@ -4696,7 +4730,7 @@
       <c r="B115" s="13"/>
       <c r="C115" s="13"/>
       <c r="D115" s="13"/>
-      <c r="E115" s="13"/>
+      <c r="E115" s="14"/>
       <c r="F115" s="13"/>
       <c r="G115" s="15"/>
     </row>
@@ -4705,7 +4739,7 @@
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
       <c r="D116" s="13"/>
-      <c r="E116" s="13"/>
+      <c r="E116" s="14"/>
       <c r="F116" s="13"/>
       <c r="G116" s="15"/>
     </row>
@@ -4714,7 +4748,7 @@
       <c r="B117" s="13"/>
       <c r="C117" s="13"/>
       <c r="D117" s="13"/>
-      <c r="E117" s="13"/>
+      <c r="E117" s="14"/>
       <c r="F117" s="13"/>
       <c r="G117" s="15"/>
     </row>
@@ -4723,7 +4757,7 @@
       <c r="B118" s="13"/>
       <c r="C118" s="13"/>
       <c r="D118" s="13"/>
-      <c r="E118" s="13"/>
+      <c r="E118" s="14"/>
       <c r="F118" s="13"/>
       <c r="G118" s="15"/>
     </row>
@@ -4732,7 +4766,7 @@
       <c r="B119" s="13"/>
       <c r="C119" s="13"/>
       <c r="D119" s="13"/>
-      <c r="E119" s="13"/>
+      <c r="E119" s="14"/>
       <c r="F119" s="13"/>
       <c r="G119" s="15"/>
     </row>
@@ -4741,7 +4775,7 @@
       <c r="B120" s="13"/>
       <c r="C120" s="13"/>
       <c r="D120" s="13"/>
-      <c r="E120" s="13"/>
+      <c r="E120" s="14"/>
       <c r="F120" s="13"/>
       <c r="G120" s="15"/>
     </row>
@@ -4750,7 +4784,7 @@
       <c r="B121" s="13"/>
       <c r="C121" s="13"/>
       <c r="D121" s="13"/>
-      <c r="E121" s="13"/>
+      <c r="E121" s="14"/>
       <c r="F121" s="13"/>
       <c r="G121" s="15"/>
     </row>
@@ -4759,7 +4793,7 @@
       <c r="B122" s="13"/>
       <c r="C122" s="13"/>
       <c r="D122" s="13"/>
-      <c r="E122" s="13"/>
+      <c r="E122" s="14"/>
       <c r="F122" s="13"/>
       <c r="G122" s="15"/>
     </row>
@@ -4768,7 +4802,7 @@
       <c r="B123" s="13"/>
       <c r="C123" s="13"/>
       <c r="D123" s="13"/>
-      <c r="E123" s="13"/>
+      <c r="E123" s="14"/>
       <c r="F123" s="13"/>
       <c r="G123" s="15"/>
     </row>
@@ -4786,7 +4820,7 @@
   <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D13" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4805,19 +4839,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -4826,10 +4860,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="11"/>
@@ -4840,10 +4874,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="11"/>
@@ -4854,10 +4888,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="11"/>
@@ -4868,10 +4902,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="11"/>
@@ -4884,13 +4918,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F6" s="11"/>
     </row>
@@ -4902,92 +4936,86 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
+    <row r="9" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
+    <row r="10" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="11"/>
@@ -5000,10 +5028,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="11"/>
@@ -5016,10 +5044,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="11"/>
@@ -5032,10 +5060,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="11"/>
@@ -5048,10 +5076,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="11"/>
@@ -5064,10 +5092,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="11"/>
@@ -5080,13 +5108,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F18" s="11"/>
     </row>
@@ -5096,13 +5124,13 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="F19" s="11"/>
     </row>
@@ -5112,10 +5140,10 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="11"/>
@@ -5126,10 +5154,10 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="11"/>
@@ -5140,10 +5168,10 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="11"/>
@@ -5154,10 +5182,10 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="11"/>
@@ -5168,10 +5196,10 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="11"/>
@@ -5182,10 +5210,10 @@
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="11"/>
@@ -5196,10 +5224,10 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="11"/>
@@ -5210,10 +5238,10 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="11"/>
@@ -5224,10 +5252,10 @@
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="11"/>
@@ -5238,10 +5266,10 @@
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="11"/>
@@ -5252,10 +5280,10 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="11"/>
@@ -5266,10 +5294,10 @@
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="11"/>
@@ -5280,10 +5308,10 @@
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="11"/>
@@ -5294,10 +5322,10 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="11"/>
@@ -5308,10 +5336,10 @@
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="11"/>
@@ -5322,10 +5350,10 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="11"/>
@@ -5336,10 +5364,10 @@
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="11"/>
@@ -5350,10 +5378,10 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="11"/>
@@ -5364,10 +5392,10 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="11"/>
@@ -5378,10 +5406,10 @@
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="11"/>
@@ -5392,10 +5420,10 @@
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="11"/>
@@ -5406,10 +5434,10 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="11"/>
@@ -5420,10 +5448,10 @@
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="11"/>
@@ -5434,10 +5462,10 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="11"/>
@@ -5448,10 +5476,10 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="11"/>
@@ -5462,10 +5490,10 @@
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="11"/>
@@ -5476,10 +5504,10 @@
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="11"/>
@@ -5490,13 +5518,13 @@
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="F47" s="11"/>
     </row>
@@ -5506,13 +5534,13 @@
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="F48" s="11"/>
     </row>
@@ -5522,13 +5550,13 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F49" s="11"/>
     </row>
@@ -5538,13 +5566,13 @@
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F50" s="11"/>
     </row>
@@ -5554,10 +5582,10 @@
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="11"/>
@@ -5567,10 +5595,10 @@
         <v>36</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="F52" s="11"/>
     </row>
@@ -5579,10 +5607,10 @@
         <v>36</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="F53" s="11"/>
     </row>
@@ -5591,10 +5619,10 @@
         <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="F54" s="11"/>
     </row>
@@ -5603,10 +5631,10 @@
         <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F55" s="11"/>
     </row>
@@ -5615,10 +5643,10 @@
         <v>36</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F56" s="11"/>
     </row>
@@ -5628,10 +5656,10 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="11"/>
@@ -5642,10 +5670,10 @@
       </c>
       <c r="B58" s="1"/>
       <c r="C58" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="11"/>
@@ -5656,10 +5684,10 @@
       </c>
       <c r="B59" s="1"/>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="11"/>
@@ -5670,10 +5698,10 @@
       </c>
       <c r="B60" s="1"/>
       <c r="C60" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="11"/>
@@ -5684,10 +5712,10 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="11"/>
@@ -5698,10 +5726,10 @@
       </c>
       <c r="B62" s="1"/>
       <c r="C62" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="11"/>
@@ -5712,10 +5740,10 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="11"/>
@@ -5726,10 +5754,10 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="11"/>
@@ -5740,10 +5768,10 @@
       </c>
       <c r="B65" s="1"/>
       <c r="C65" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="11"/>
@@ -5754,10 +5782,10 @@
       </c>
       <c r="B66" s="1"/>
       <c r="C66" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="11"/>
@@ -5768,10 +5796,10 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="11"/>
@@ -5782,10 +5810,10 @@
       </c>
       <c r="B68" s="1"/>
       <c r="C68" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="11"/>
@@ -5795,10 +5823,10 @@
         <v>36</v>
       </c>
       <c r="C69" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F69" s="11"/>
     </row>
@@ -5808,10 +5836,10 @@
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="11"/>
@@ -5822,10 +5850,10 @@
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="11"/>
@@ -5836,10 +5864,10 @@
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="11"/>
@@ -5850,10 +5878,10 @@
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="11"/>
@@ -5864,10 +5892,10 @@
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="11"/>
@@ -5878,10 +5906,10 @@
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="11"/>
@@ -5892,10 +5920,10 @@
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="11"/>
@@ -5906,10 +5934,10 @@
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="11"/>
@@ -5920,10 +5948,10 @@
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="11"/>
@@ -5934,10 +5962,10 @@
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="11"/>
@@ -5948,10 +5976,10 @@
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="11"/>
@@ -5962,10 +5990,10 @@
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="11"/>
@@ -5976,10 +6004,10 @@
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="11"/>
@@ -5990,10 +6018,10 @@
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="11"/>
@@ -6004,10 +6032,10 @@
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="11"/>
@@ -6018,10 +6046,10 @@
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="11"/>
@@ -6032,10 +6060,10 @@
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="11"/>
@@ -6046,10 +6074,10 @@
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="11"/>
@@ -6060,10 +6088,10 @@
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="11"/>
@@ -6074,10 +6102,10 @@
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="11"/>
@@ -6088,10 +6116,10 @@
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="11"/>
@@ -6102,13 +6130,13 @@
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="F91" s="11"/>
     </row>
@@ -6118,10 +6146,10 @@
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="11"/>
@@ -6132,10 +6160,10 @@
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="11"/>
@@ -6146,10 +6174,10 @@
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="11"/>
@@ -6160,10 +6188,10 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="11"/>
@@ -6174,10 +6202,10 @@
       </c>
       <c r="B96" s="1"/>
       <c r="C96" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="11"/>
@@ -6188,10 +6216,10 @@
       </c>
       <c r="B97" s="1"/>
       <c r="C97" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="11"/>
@@ -6202,10 +6230,10 @@
       </c>
       <c r="B98" s="1"/>
       <c r="C98" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="11"/>
@@ -6216,10 +6244,10 @@
       </c>
       <c r="B99" s="1"/>
       <c r="C99" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="11"/>
@@ -6230,10 +6258,10 @@
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="11"/>
@@ -6244,10 +6272,10 @@
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="11"/>
@@ -6258,10 +6286,10 @@
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="11"/>
@@ -6272,10 +6300,10 @@
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="11"/>
@@ -6501,7 +6529,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6520,22 +6548,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -6543,20 +6571,24 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="9" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="6"/>
+      <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
@@ -7123,7 +7155,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7142,22 +7174,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -7165,13 +7197,13 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="9" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="G2" s="7"/>
     </row>
@@ -7180,10 +7212,10 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="9" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -7193,10 +7225,10 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="9" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -7206,10 +7238,10 @@
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="9" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -7219,10 +7251,10 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -7232,10 +7264,10 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -7245,10 +7277,10 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -7258,23 +7290,23 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -7283,17 +7315,25 @@
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="6"/>
+      <c r="D11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="6"/>
+      <c r="D12" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
@@ -7800,28 +7840,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
@@ -7830,16 +7870,16 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="17" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="I2" s="19"/>
     </row>
@@ -8558,22 +8598,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -8581,10 +8621,10 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>

</xml_diff>

<commit_message>
230408 View all Creez Find by Id Adaug Remainder
230407
I tried to use lombok but I couldn't because is hard to integrate lombok with mapstruct and the Id shall be ignored.
I managed to rebase but I lost all modifications
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="660" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB68CD1-CF0F-4EC9-8479-67396438FF3B}"/>
+  <xr:revisionPtr revIDLastSave="717" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DA4A3F3-1EBA-4BB0-8C67-83B1230B8444}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="142">
   <si>
     <t>N</t>
   </si>
@@ -519,6 +519,51 @@
   </si>
   <si>
     <t>Before tasks a cercal progress bar</t>
+  </si>
+  <si>
+    <t>By User</t>
+  </si>
+  <si>
+    <t>Trebuie sa se caute in lista de useri nu dupa cine a create(trebuie sa verific ca am implementat asta peste tot)</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Trebuie sa verific toate queriile dupa refacturare de la plurar la singular</t>
+  </si>
+  <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>Toate elementele trebuie sa aiba un creator(verifica ca ii asa la toate)</t>
+  </si>
+  <si>
+    <t>Un remainder are un singur user creator, daca se doreste ca acest remainder sa apara si la alti useri atunci se va crea un nou creator</t>
+  </si>
+  <si>
+    <t>Mapper</t>
+  </si>
+  <si>
+    <t>Refactor all mapper from pliural to list</t>
+  </si>
+  <si>
+    <t>Theow exception</t>
+  </si>
+  <si>
+    <t>where is batter to throw excception
+in service ca nu are rost sa mergi cu calculel mai departe daca nu este o exceptie
+in controller ca este ultimul loc unde unde il avem de facut si acoo poate mai putem sa avem si null 
+sau sa folosesc un try catch in service?</t>
+  </si>
+  <si>
+    <t>Intellij user to string view</t>
+  </si>
+  <si>
+    <t>imi apare err cand afisez useru ca imi face user in user</t>
   </si>
 </sst>
 </file>
@@ -600,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -648,6 +693,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1799,6 +1847,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
@@ -1860,7 +1912,7 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:F130">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:F130">
     <sortCondition ref="A1:A130"/>
   </sortState>
   <tableColumns count="6">
@@ -2253,7 +2305,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,11 +2374,17 @@
       </c>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
+      <c r="B5" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4820,7 +4878,7 @@
   <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D14"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4911,9 +4969,7 @@
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -4929,9 +4985,7 @@
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -4989,9 +5043,7 @@
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>4</v>
       </c>
@@ -5005,9 +5057,7 @@
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>5</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>4</v>
       </c>
@@ -5022,205 +5072,201 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>7</v>
-      </c>
+    <row r="14" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E14" s="20"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>8</v>
-      </c>
+    <row r="15" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E15" s="20"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>9</v>
-      </c>
+    <row r="16" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="E16" s="20"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>10</v>
-      </c>
+    <row r="17" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="E17" s="20"/>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E18" s="20"/>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>12</v>
-      </c>
-      <c r="B19" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E19" s="20"/>
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="E20" s="20"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="E21" s="20"/>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>132</v>
+      </c>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="E25" s="20"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -5229,77 +5275,77 @@
       <c r="D26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="20"/>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E27" s="20"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E30" s="20"/>
       <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="E31" s="20"/>
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5311,9 +5357,9 @@
         <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E32" s="20"/>
       <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5325,9 +5371,9 @@
         <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E33" s="20"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5339,9 +5385,9 @@
         <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="E34" s="20"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5353,9 +5399,9 @@
         <v>16</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="E35" s="20"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5367,37 +5413,37 @@
         <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="E36" s="20"/>
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E37" s="20"/>
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="E38" s="20"/>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5409,9 +5455,9 @@
         <v>55</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E39" s="20"/>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5423,9 +5469,9 @@
         <v>55</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="E40" s="20"/>
       <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5437,9 +5483,9 @@
         <v>55</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E41" s="20"/>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5451,9 +5497,9 @@
         <v>55</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="E42" s="20"/>
       <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5465,9 +5511,9 @@
         <v>55</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E43" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="E43" s="20"/>
       <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5479,9 +5525,9 @@
         <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E44" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="E44" s="20"/>
       <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5493,9 +5539,9 @@
         <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E45" s="20"/>
       <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5507,9 +5553,9 @@
         <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E46" s="20"/>
       <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5521,11 +5567,9 @@
         <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E47" s="20"/>
       <c r="F47" s="11"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5537,11 +5581,9 @@
         <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E48" s="20"/>
       <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5553,10 +5595,10 @@
         <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="F49" s="11"/>
     </row>
@@ -5569,10 +5611,10 @@
         <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="F50" s="11"/>
     </row>
@@ -5585,33 +5627,41 @@
         <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F51" s="11"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>35</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F52" s="11"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>35</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="11"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>36</v>
-      </c>
-      <c r="C52" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F52" s="11"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>36</v>
-      </c>
-      <c r="C53" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="E53" s="20"/>
       <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5622,8 +5672,9 @@
         <v>81</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>82</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E54" s="3"/>
       <c r="F54" s="11"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5634,8 +5685,9 @@
         <v>81</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E55" s="3"/>
       <c r="F55" s="11"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5646,36 +5698,35 @@
         <v>81</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E56" s="3"/>
       <c r="F56" s="11"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>36</v>
       </c>
-      <c r="B57" s="1"/>
       <c r="C57" t="s">
         <v>81</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E57" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E57" s="3"/>
       <c r="F57" s="11"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>36</v>
       </c>
-      <c r="B58" s="1"/>
       <c r="C58" t="s">
         <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E58" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="E58" s="3"/>
       <c r="F58" s="11"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5687,9 +5738,9 @@
         <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E59" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="E59" s="20"/>
       <c r="F59" s="11"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5701,9 +5752,9 @@
         <v>81</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E60" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="E60" s="20"/>
       <c r="F60" s="11"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5715,9 +5766,9 @@
         <v>81</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E61" s="20"/>
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5729,9 +5780,9 @@
         <v>81</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E62" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E62" s="20"/>
       <c r="F62" s="11"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5743,9 +5794,9 @@
         <v>81</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E63" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="E63" s="20"/>
       <c r="F63" s="11"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5757,9 +5808,9 @@
         <v>81</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E64" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E64" s="20"/>
       <c r="F64" s="11"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5771,9 +5822,9 @@
         <v>81</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E65" s="20"/>
       <c r="F65" s="11"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5785,9 +5836,9 @@
         <v>81</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E66" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="E66" s="20"/>
       <c r="F66" s="11"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5799,9 +5850,9 @@
         <v>81</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E67" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="E67" s="20"/>
       <c r="F67" s="11"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5813,49 +5864,50 @@
         <v>81</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E68" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="E68" s="20"/>
       <c r="F68" s="11"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>36</v>
       </c>
+      <c r="B69" s="1"/>
       <c r="C69" t="s">
         <v>81</v>
       </c>
       <c r="D69" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E69" s="20"/>
+      <c r="F69" s="11"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>36</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" t="s">
+        <v>81</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" s="20"/>
+      <c r="F70" s="11"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>36</v>
+      </c>
+      <c r="C71" t="s">
+        <v>81</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F69" s="11"/>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>37</v>
-      </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="11"/>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>37</v>
-      </c>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E71" s="1"/>
+      <c r="E71" s="3"/>
       <c r="F71" s="11"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5867,9 +5919,9 @@
         <v>83</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E72" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E72" s="20"/>
       <c r="F72" s="11"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5881,9 +5933,9 @@
         <v>83</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E73" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E73" s="20"/>
       <c r="F73" s="11"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5895,9 +5947,9 @@
         <v>83</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E74" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="E74" s="20"/>
       <c r="F74" s="11"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5909,9 +5961,9 @@
         <v>83</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E75" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E75" s="20"/>
       <c r="F75" s="11"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5923,9 +5975,9 @@
         <v>83</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E76" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="E76" s="20"/>
       <c r="F76" s="11"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5937,9 +5989,9 @@
         <v>83</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E77" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="E77" s="20"/>
       <c r="F77" s="11"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5951,9 +6003,9 @@
         <v>83</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E78" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="E78" s="20"/>
       <c r="F78" s="11"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5965,9 +6017,9 @@
         <v>83</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E79" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E79" s="20"/>
       <c r="F79" s="11"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5979,9 +6031,9 @@
         <v>83</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E80" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E80" s="20"/>
       <c r="F80" s="11"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5993,9 +6045,9 @@
         <v>83</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E81" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="E81" s="20"/>
       <c r="F81" s="11"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6007,9 +6059,9 @@
         <v>83</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E82" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="E82" s="20"/>
       <c r="F82" s="11"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6021,9 +6073,9 @@
         <v>83</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E83" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E83" s="20"/>
       <c r="F83" s="11"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6035,9 +6087,9 @@
         <v>83</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E84" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="E84" s="20"/>
       <c r="F84" s="11"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6049,9 +6101,9 @@
         <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E85" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="E85" s="20"/>
       <c r="F85" s="11"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6063,9 +6115,9 @@
         <v>83</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E86" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="E86" s="20"/>
       <c r="F86" s="11"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6077,37 +6129,37 @@
         <v>83</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E87" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E87" s="20"/>
       <c r="F87" s="11"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E88" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="E88" s="20"/>
       <c r="F88" s="11"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E89" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="E89" s="20"/>
       <c r="F89" s="11"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6119,12 +6171,12 @@
         <v>13</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E90" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E90" s="20"/>
       <c r="F90" s="11"/>
     </row>
-    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>41</v>
       </c>
@@ -6133,39 +6185,39 @@
         <v>13</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>91</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E91" s="20"/>
       <c r="F91" s="11"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E92" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="E92" s="20"/>
       <c r="F92" s="11"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E93" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="E93" s="20" t="s">
+        <v>91</v>
+      </c>
       <c r="F93" s="11"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6177,9 +6229,9 @@
         <v>55</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E94" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E94" s="20"/>
       <c r="F94" s="11"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6191,37 +6243,37 @@
         <v>55</v>
       </c>
       <c r="D95" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E95" s="20"/>
+      <c r="F95" s="11"/>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>42</v>
+      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E96" s="20"/>
+      <c r="F96" s="11"/>
+    </row>
+    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>42</v>
+      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E95" s="1"/>
-      <c r="F95" s="11"/>
-    </row>
-    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>43</v>
-      </c>
-      <c r="B96" s="1"/>
-      <c r="C96" t="s">
-        <v>81</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E96" s="1"/>
-      <c r="F96" s="11"/>
-    </row>
-    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>43</v>
-      </c>
-      <c r="B97" s="1"/>
-      <c r="C97" t="s">
-        <v>81</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E97" s="1"/>
+      <c r="E97" s="20"/>
       <c r="F97" s="11"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6233,9 +6285,9 @@
         <v>81</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E98" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E98" s="20"/>
       <c r="F98" s="11"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6247,37 +6299,37 @@
         <v>81</v>
       </c>
       <c r="D99" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E99" s="20"/>
+      <c r="F99" s="11"/>
+    </row>
+    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>43</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" t="s">
+        <v>81</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E100" s="20"/>
+      <c r="F100" s="11"/>
+    </row>
+    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>43</v>
+      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" t="s">
+        <v>81</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E99" s="1"/>
-      <c r="F99" s="11"/>
-    </row>
-    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>44</v>
-      </c>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E100" s="1"/>
-      <c r="F100" s="11"/>
-    </row>
-    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>44</v>
-      </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E101" s="1"/>
+      <c r="E101" s="20"/>
       <c r="F101" s="11"/>
     </row>
     <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6289,9 +6341,9 @@
         <v>83</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E102" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E102" s="20"/>
       <c r="F102" s="11"/>
     </row>
     <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6303,25 +6355,37 @@
         <v>83</v>
       </c>
       <c r="D103" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E103" s="20"/>
+      <c r="F103" s="11"/>
+    </row>
+    <row r="104" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>44</v>
+      </c>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E104" s="20"/>
+      <c r="F104" s="11"/>
+    </row>
+    <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>44</v>
+      </c>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E103" s="1"/>
-      <c r="F103" s="11"/>
-    </row>
-    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="11"/>
-    </row>
-    <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
+      <c r="E105" s="20"/>
       <c r="F105" s="11"/>
     </row>
     <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6329,7 +6393,7 @@
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
+      <c r="E106" s="20"/>
       <c r="F106" s="11"/>
     </row>
     <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6337,13 +6401,15 @@
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
+      <c r="E107" s="20"/>
       <c r="F107" s="11"/>
     </row>
     <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E108" s="3"/>
       <c r="F108" s="11"/>
     </row>
     <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E109" s="3"/>
       <c r="F109" s="11"/>
     </row>
     <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6351,7 +6417,7 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
+      <c r="E110" s="20"/>
       <c r="F110" s="11"/>
     </row>
     <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6359,7 +6425,7 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
+      <c r="E111" s="20"/>
       <c r="F111" s="11"/>
     </row>
     <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6367,7 +6433,7 @@
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
+      <c r="E112" s="20"/>
       <c r="F112" s="11"/>
     </row>
     <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6375,7 +6441,7 @@
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
+      <c r="E113" s="20"/>
       <c r="F113" s="11"/>
     </row>
     <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6383,7 +6449,7 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
+      <c r="E114" s="20"/>
       <c r="F114" s="11"/>
     </row>
     <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6391,7 +6457,7 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
+      <c r="E115" s="20"/>
       <c r="F115" s="11"/>
     </row>
     <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6399,7 +6465,7 @@
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
+      <c r="E116" s="20"/>
       <c r="F116" s="11"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6407,7 +6473,7 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
+      <c r="E117" s="20"/>
       <c r="F117" s="11"/>
     </row>
     <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6415,7 +6481,7 @@
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
+      <c r="E118" s="20"/>
       <c r="F118" s="11"/>
     </row>
     <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6423,7 +6489,7 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
+      <c r="E119" s="20"/>
       <c r="F119" s="11"/>
     </row>
     <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6431,7 +6497,7 @@
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
+      <c r="E120" s="20"/>
       <c r="F120" s="11"/>
     </row>
     <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6439,7 +6505,7 @@
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
+      <c r="E121" s="20"/>
       <c r="F121" s="11"/>
     </row>
     <row r="122" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6447,7 +6513,7 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
+      <c r="E122" s="20"/>
       <c r="F122" s="11"/>
     </row>
     <row r="123" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6455,7 +6521,7 @@
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
+      <c r="E123" s="20"/>
       <c r="F123" s="11"/>
     </row>
     <row r="124" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6463,7 +6529,7 @@
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
+      <c r="E124" s="20"/>
       <c r="F124" s="11"/>
     </row>
     <row r="125" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6471,7 +6537,7 @@
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
+      <c r="E125" s="20"/>
       <c r="F125" s="11"/>
     </row>
     <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6479,7 +6545,7 @@
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
-      <c r="E126" s="1"/>
+      <c r="E126" s="20"/>
       <c r="F126" s="11"/>
     </row>
     <row r="127" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6487,7 +6553,7 @@
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
+      <c r="E127" s="20"/>
       <c r="F127" s="11"/>
     </row>
     <row r="128" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6495,7 +6561,7 @@
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
+      <c r="E128" s="20"/>
       <c r="F128" s="11"/>
     </row>
     <row r="129" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6503,7 +6569,7 @@
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
+      <c r="E129" s="20"/>
       <c r="F129" s="11"/>
     </row>
     <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6511,7 +6577,7 @@
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
+      <c r="E130" s="20"/>
       <c r="F130" s="11"/>
     </row>
   </sheetData>
@@ -7154,8 +7220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE23E348-29D0-4FF8-A4A5-A0998E1F2F1A}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7337,21 +7403,29 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="6"/>
+      <c r="D14" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>134</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
@@ -7359,17 +7433,25 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="6"/>
+      <c r="D15" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="6"/>
+      <c r="D16" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
@@ -7377,8 +7459,12 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>

</xml_diff>

<commit_message>
reformatting checking for note
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="762" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92959524-65A9-40CC-B806-DCC9795811C8}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81C74410-4492-4847-9472-8A818646A474}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Idee" sheetId="8" r:id="rId2"/>
     <sheet name="Neclar" sheetId="16" r:id="rId3"/>
-    <sheet name="CodingRoles" sheetId="11" r:id="rId4"/>
-    <sheet name="Implement" sheetId="2" r:id="rId5"/>
-    <sheet name="Learn" sheetId="14" r:id="rId6"/>
-    <sheet name="BE_todo" sheetId="4" r:id="rId7"/>
-    <sheet name="BE_test" sheetId="13" r:id="rId8"/>
-    <sheet name="FE_todo" sheetId="6" r:id="rId9"/>
+    <sheet name="DB" sheetId="17" r:id="rId4"/>
+    <sheet name="CodingRoles" sheetId="11" r:id="rId5"/>
+    <sheet name="Implement" sheetId="2" r:id="rId6"/>
+    <sheet name="Learn" sheetId="14" r:id="rId7"/>
+    <sheet name="BE_todo" sheetId="4" r:id="rId8"/>
+    <sheet name="BE_test" sheetId="13" r:id="rId9"/>
+    <sheet name="FE_todo" sheetId="6" r:id="rId10"/>
+    <sheet name="Review" sheetId="19" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -155,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="181">
   <si>
     <t>N</t>
   </si>
@@ -629,6 +631,101 @@
     <t>Recapitulare exceptii
 Unde ar fi mai bine sa definesc exceptiile in service sau in controller
 Cum se vad exceptiile in controller</t>
+  </si>
+  <si>
+    <t>Add User in userlist</t>
+  </si>
+  <si>
+    <t>cand fac post adaug userul la userlis
+cand caut dupa use sa caut dupa useri din userlist</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Fild</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Descriere</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>userList</t>
+  </si>
+  <si>
+    <t>creatorul</t>
+  </si>
+  <si>
+    <t>users that have access to the note</t>
+  </si>
+  <si>
+    <t>Adaug userul la in lista la constructie
+Share-uesc cu un alt user lista</t>
+  </si>
+  <si>
+    <t>Add user to userlist</t>
+  </si>
+  <si>
+    <t>share with another user</t>
+  </si>
+  <si>
+    <t>User list of user</t>
+  </si>
+  <si>
+    <t>A useer have a user list to can share easyer informations  without searching only piknig from the list</t>
+  </si>
+  <si>
+    <t>Ar trebui sa pun aceste checks intr-o clasa?</t>
+  </si>
+  <si>
+    <t>Am gandit bine traba asta cu Exceptiile ?</t>
+  </si>
+  <si>
+    <t>Nu a mers sa folosesc si lombok si mapstruct</t>
+  </si>
+  <si>
+    <t>Cum ar trebui sa folosesc eu gitHub pentru proiectul asta?</t>
+  </si>
+  <si>
+    <t>Delete user from Userlist</t>
+  </si>
+  <si>
+    <t>Delete user form user</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Check is in loc de is</t>
+  </si>
+  <si>
+    <t>Trebuie sa las verificarea inainte sa adauga pentru ca chiar daca in frontend se face verificare o data cand se adauga se poate modifica baza de date si sar putea sa avem o problema incerc sa adug ceva care intre timp a fost sters</t>
+  </si>
+  <si>
+    <t>Da asa ar fi util</t>
+  </si>
+  <si>
+    <t>cam da dar se mai poate utiliza un pic</t>
+  </si>
+  <si>
+    <t>React native Ionic</t>
+  </si>
+  <si>
+    <t>Rename class</t>
+  </si>
+  <si>
+    <t>checkIfIsAndOrLiked</t>
   </si>
 </sst>
 </file>
@@ -710,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -762,11 +859,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="102">
     <dxf>
       <font>
         <strike val="0"/>
@@ -775,12 +875,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -790,12 +889,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -805,12 +903,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -820,12 +918,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -839,12 +936,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -854,12 +950,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -869,12 +964,25 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -889,7 +997,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1730,6 +1837,299 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -2010,12 +2410,12 @@
       </font>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="Table Style 1" defaultPivotStyle="PivotStyleMedium9">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="4" xr9:uid="{803E0FE5-88DA-4CC3-8742-6FED218BE0BD}">
-      <tableStyleElement type="wholeTable" dxfId="81"/>
-      <tableStyleElement type="headerRow" dxfId="80"/>
-      <tableStyleElement type="firstRowStripe" dxfId="79"/>
-      <tableStyleElement type="secondRowStripe" dxfId="78"/>
+      <tableStyleElement type="wholeTable" dxfId="101"/>
+      <tableStyleElement type="headerRow" dxfId="100"/>
+      <tableStyleElement type="firstRowStripe" dxfId="99"/>
+      <tableStyleElement type="secondRowStripe" dxfId="98"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2036,82 +2436,137 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+  <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2AB95F0A-997C-4A60-893A-C402C47724DF}" name="N" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{F6E15414-A725-4A88-94CE-0137EFE7B8F6}" name="Categorie" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{EEE22B11-7605-42D0-9695-0D9B47D4122C}" name="S" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{BF71001F-F5F6-4A8F-9314-E52756A5E54C}" name="Actiune" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{BDD7A213-BDAC-48B4-829D-524419C42642}" name="Column1" dataDxfId="91"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
-  <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2AB95F0A-997C-4A60-893A-C402C47724DF}" name="N" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{F6E15414-A725-4A88-94CE-0137EFE7B8F6}" name="Categorie" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{EEE22B11-7605-42D0-9695-0D9B47D4122C}" name="S" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{BF71001F-F5F6-4A8F-9314-E52756A5E54C}" name="Actiune" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{BDD7A213-BDAC-48B4-829D-524419C42642}" name="Column1" dataDxfId="71"/>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A1D70E3-5294-4928-A968-C76C79402048}" name="Table1345" displayName="Table1345" ref="A1:G64" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
+    <sortCondition ref="D1:D64"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8EA2D119-3E27-4566-81D1-1306D8CC3651}" name="N" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{65E039F8-B443-4BD3-BD08-BB9C9AB39762}" name="O" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{C722F227-4153-4370-8D0B-BC8BD2702337}" name="S" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{F0C8AA5A-2740-4F1F-B7C4-BEAC7C4B8938}" name="Categorie" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{E40C8687-72DF-46F5-A761-A03AFAA63494}" name="Todo" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{4D62348B-CDB2-403B-B07F-3DAD12C60F4C}" name="Done" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{CEF8DE16-2E80-4774-AB3E-CC177F386B65}" name="Other" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3F1CF4E8-4B34-4538-86A1-924888B706AA}" name="Table134512" displayName="Table134512" ref="A1:G64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
+    <sortCondition ref="D1:D64"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{A85BEFF4-BA3A-4B54-9E56-29A6C8034025}" name="N" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{4A9D7FEB-9DBB-4795-B721-103BD99A4ADF}" name="O" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{FC91FAFD-E4A0-4389-BCC6-36C43FA2DFF9}" name="S" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{17BB3042-2571-48EF-942E-9CD7A3E2311A}" name="Categorie" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F883D474-6801-4AF7-8666-98FE9DE794B9}" name="Todo" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{C6D0FB08-CD80-4E52-8F39-672B61996C20}" name="Done" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{6257895A-4251-476F-8549-E26723B65ABE}" name="Other" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96D400E0-6F3A-4A4F-B7B3-1DDE9DC0092F}" name="Table136" displayName="Table136" ref="A1:F123" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96D400E0-6F3A-4A4F-B7B3-1DDE9DC0092F}" name="Table136" displayName="Table136" ref="A1:F123" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
   <autoFilter ref="A1:F123" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E123">
     <sortCondition ref="A1:A123"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D7628B32-36E1-4AAD-BCC2-DBE15AE3A288}" name="N" dataDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{92E6ACD6-AC10-432E-B149-97C9B4FF93DB}" name="S" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{46DA51A3-0AFC-4BAD-90AC-BC1D0B4EB350}" name="Subiect" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{0E9011E1-5C6D-4EA0-8863-54B6CD6F951A}" name="Idee" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{040BA331-0196-4FE3-9159-98587F54059B}" name="Detalii" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{6A1A050C-85AA-4B4D-824C-8D2F5BB52A8C}" name="Altele" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{D7628B32-36E1-4AAD-BCC2-DBE15AE3A288}" name="N" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{92E6ACD6-AC10-432E-B149-97C9B4FF93DB}" name="S" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{46DA51A3-0AFC-4BAD-90AC-BC1D0B4EB350}" name="Subiect" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{0E9011E1-5C6D-4EA0-8863-54B6CD6F951A}" name="Idee" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{040BA331-0196-4FE3-9159-98587F54059B}" name="Detalii" dataDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{6A1A050C-85AA-4B4D-824C-8D2F5BB52A8C}" name="Altele" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6F2DB8FF-9816-4330-A6E4-F6AD4DF22B7B}" name="Table13610" displayName="Table13610" ref="A1:F123" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6F2DB8FF-9816-4330-A6E4-F6AD4DF22B7B}" name="Table13610" displayName="Table13610" ref="A1:F123" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
   <autoFilter ref="A1:F123" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E123">
     <sortCondition ref="A1:A123"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5CDA0D29-521C-41E5-A387-3AF6714FFBE5}" name="N" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{3B1BEDED-8952-449C-A09C-FF9332F35904}" name="S" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{469B214E-CE09-435C-89F7-6A3718BE05D6}" name="Subiect" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{CE3184A5-0D4E-439A-8F3D-9DA6F83F9EEC}" name="Problema" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B0CDF7B6-08BB-42E1-8811-28D412074EE5}" name="Detalii" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{9FC5F15B-2AC7-4945-9DFF-099EFA301400}" name="Altele" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5CDA0D29-521C-41E5-A387-3AF6714FFBE5}" name="N" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{3B1BEDED-8952-449C-A09C-FF9332F35904}" name="S" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{469B214E-CE09-435C-89F7-6A3718BE05D6}" name="Subiect" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{CE3184A5-0D4E-439A-8F3D-9DA6F83F9EEC}" name="Problema" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{B0CDF7B6-08BB-42E1-8811-28D412074EE5}" name="Detalii" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{9FC5F15B-2AC7-4945-9DFF-099EFA301400}" name="Altele" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7AE42CCE-2F3D-4A2D-9A64-D811029D5849}" name="Table1367" displayName="Table1367" ref="A1:G123" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
-  <autoFilter ref="A1:G123" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F123">
-    <sortCondition ref="A1:A123"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7A1E696C-7320-4ED1-BB70-E1E1E76934B7}" name="Table13411" displayName="Table13411" ref="A1:I64" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+  <autoFilter ref="A1:I64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
+    <sortCondition ref="D1:D64"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D39497DB-A5B1-405C-ABF9-784FB5093D9E}" name="N" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{552B6E2B-C748-4592-80A6-F06198265568}" name="S" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{CA6589DF-F818-4280-A795-D9B613C17207}" name="Categori" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{A76965F2-410F-483F-A5C7-C28DF80869A7}" name="Subiect" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{77866754-F604-4AFD-B30F-0B9B42069010}" name="Idee" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{007A6C76-1734-4E52-A225-11FD9E282AD5}" name="Detalii" dataDxfId="55"/>
-    <tableColumn id="6" xr3:uid="{27A6BDE0-42B2-453A-B22C-FCBE2C639359}" name="Altele" dataDxfId="54"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{B48B7FAB-BC79-4D4C-8CED-E59F89652CDA}" name="N" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{613FDC02-888C-4ABF-97AC-E6C21190082B}" name="O" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{21324744-5AB4-4E0B-8AE2-9FE4BFD48BFB}" name="S" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{D7A7BC81-4DB7-440D-8502-B491EEA5A63E}" name="Entity" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{CBEC9E30-A0B7-4EF8-8412-00461DB28944}" name="Fild" dataDxfId="68"/>
+    <tableColumn id="8" xr3:uid="{11D02E52-5C1A-4903-9553-6C26004686E9}" name="Type" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{7A5BEC6B-B4D8-4833-83B4-8B7643195A0B}" name="Descriere" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{CC2AC36D-7199-4603-8C1E-62928752F700}" name="Column1" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{89D64582-B0D4-4D98-BDFC-33359A15B946}" name="Other" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F131" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:F131" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7AE42CCE-2F3D-4A2D-9A64-D811029D5849}" name="Table1367" displayName="Table1367" ref="A1:G123" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+  <autoFilter ref="A1:G123" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F123">
+    <sortCondition ref="A1:A123"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{D39497DB-A5B1-405C-ABF9-784FB5093D9E}" name="N" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{552B6E2B-C748-4592-80A6-F06198265568}" name="S" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{CA6589DF-F818-4280-A795-D9B613C17207}" name="Categori" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{A76965F2-410F-483F-A5C7-C28DF80869A7}" name="Subiect" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{77866754-F604-4AFD-B30F-0B9B42069010}" name="Idee" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{007A6C76-1734-4E52-A225-11FD9E282AD5}" name="Detalii" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{27A6BDE0-42B2-453A-B22C-FCBE2C639359}" name="Altele" dataDxfId="55"/>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F133" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:F133" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
     <filterColumn colId="1">
       <filters blank="1">
         <filter val="0"/>
@@ -2120,94 +2575,75 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:F131">
-    <sortCondition ref="B1:B131"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:F133">
+    <sortCondition ref="B1:B133"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{867A761B-88B0-4ABF-B456-C4E8879A3300}" name="S" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{D3CD6840-B70C-43CD-9CAB-43DF78DC5F53}" name="Clasa" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{BDAD06C9-1E35-4E06-9E0A-F8976EF9241F}" name="Actiune" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{10F82FD2-FA3B-4744-9F8E-8BBF8086317C}" name="Lucru" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{90DACBD6-382A-4516-9493-642A496B48A3}" name="Other" dataDxfId="46"/>
-  </tableColumns>
-  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B9E3B11C-1970-4BFF-A50E-74D52AF99C97}" name="Table1349" displayName="Table1349" ref="A1:G64" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
-  <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
-    <sortCondition ref="D1:D64"/>
-  </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AAC6E595-E99D-4DB1-90E5-47DC31EECFA8}" name="N" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{001B6DB2-FA88-4CB6-B9E6-565C4EA7654F}" name="O" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{E4011D19-60DB-47C2-966A-2D32DC442A47}" name="S" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{B695BADD-9DBE-47D9-BA56-ED21B92A1828}" name="Categorie" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{3D686112-17E6-42F3-89F6-BC315ABBA6D6}" name="Todo" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{6783A8A6-9E60-465A-8F8C-E3458EA428FD}" name="Done" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{735045F8-2FCE-4A18-99FF-9394759A9FCA}" name="Other" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{867A761B-88B0-4ABF-B456-C4E8879A3300}" name="S" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{D3CD6840-B70C-43CD-9CAB-43DF78DC5F53}" name="Clasa" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{BDAD06C9-1E35-4E06-9E0A-F8976EF9241F}" name="Actiune" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{10F82FD2-FA3B-4744-9F8E-8BBF8086317C}" name="Lucru" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{90DACBD6-382A-4516-9493-642A496B48A3}" name="Other" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8BA42F9-DFED-45EA-AC41-6E0B5C9E450B}" name="Table134" displayName="Table134" ref="A1:G64" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B9E3B11C-1970-4BFF-A50E-74D52AF99C97}" name="Table1349" displayName="Table1349" ref="A1:G64" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4AC187AE-6AE2-4BEB-B499-A17E030775F3}" name="N" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{26157288-6E0E-4622-B6FF-6D7FCEA74C7F}" name="O" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{E3D3E698-5804-466F-B57A-35EE00DDB50F}" name="S" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{06199DE7-502A-4366-9BE0-434E4102843E}" name="Categorie" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{905CDAB0-DBAC-4C66-84D2-333728828DA0}" name="Todo" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{8AA007C0-EF3A-49CD-9337-10E6C19D0A5A}" name="Done" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{CF3AF89B-CD81-4A43-B444-E6F531918673}" name="Other" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{AAC6E595-E99D-4DB1-90E5-47DC31EECFA8}" name="N" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{001B6DB2-FA88-4CB6-B9E6-565C4EA7654F}" name="O" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{E4011D19-60DB-47C2-966A-2D32DC442A47}" name="S" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{B695BADD-9DBE-47D9-BA56-ED21B92A1828}" name="Categorie" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{3D686112-17E6-42F3-89F6-BC315ABBA6D6}" name="Todo" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{6783A8A6-9E60-465A-8F8C-E3458EA428FD}" name="Done" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{735045F8-2FCE-4A18-99FF-9394759A9FCA}" name="Other" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C98A4A27-05C0-44E7-9CF2-3E94DCEAB4D7}" name="Table1348" displayName="Table1348" ref="A1:I64" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:I64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D8BA42F9-DFED-45EA-AC41-6E0B5C9E450B}" name="Table134" displayName="Table134" ref="A1:G64" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="D1:D64"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FB6440A4-99DA-4E49-AA03-808FA3189E2D}" name="N" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{31A17B15-80EB-42E1-A5A0-335529E67891}" name="O" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{D7C50E10-7A63-4D98-961E-CEBC519A4F3A}" name="S" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{4929AF3D-E527-44F8-83E4-6AE5FF5BA752}" name="Categorie" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{160D8024-BF24-4D71-A879-3001AEF28DB0}" name="Scop" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{68958FAA-582A-40BC-88E4-DFEFCD085D7D}" name="Given" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{58D080F2-3A38-4170-A080-888A61E6472D}" name="When" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{D820C683-EACB-473E-8174-BDFBE5643443}" name="Then" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{FE5DB5B8-32DD-4A39-8CE0-9093E1EA1F43}" name="Other" dataDxfId="17"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{4AC187AE-6AE2-4BEB-B499-A17E030775F3}" name="N" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{26157288-6E0E-4622-B6FF-6D7FCEA74C7F}" name="O" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{E3D3E698-5804-466F-B57A-35EE00DDB50F}" name="S" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{06199DE7-502A-4366-9BE0-434E4102843E}" name="Categorie" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{905CDAB0-DBAC-4C66-84D2-333728828DA0}" name="Todo" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{8AA007C0-EF3A-49CD-9337-10E6C19D0A5A}" name="Done" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{CF3AF89B-CD81-4A43-B444-E6F531918673}" name="Other" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A1D70E3-5294-4928-A968-C76C79402048}" name="Table1345" displayName="Table1345" ref="A1:G64" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:G64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C98A4A27-05C0-44E7-9CF2-3E94DCEAB4D7}" name="Table1348" displayName="Table1348" ref="A1:I64" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:I64" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F64">
     <sortCondition ref="D1:D64"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8EA2D119-3E27-4566-81D1-1306D8CC3651}" name="N" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{65E039F8-B443-4BD3-BD08-BB9C9AB39762}" name="O" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{C722F227-4153-4370-8D0B-BC8BD2702337}" name="S" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{F0C8AA5A-2740-4F1F-B7C4-BEAC7C4B8938}" name="Categorie" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{E40C8687-72DF-46F5-A761-A03AFAA63494}" name="Todo" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4D62348B-CDB2-403B-B07F-3DAD12C60F4C}" name="Done" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{CEF8DE16-2E80-4774-AB3E-CC177F386B65}" name="Other" dataDxfId="8"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{FB6440A4-99DA-4E49-AA03-808FA3189E2D}" name="N" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{31A17B15-80EB-42E1-A5A0-335529E67891}" name="O" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{D7C50E10-7A63-4D98-961E-CEBC519A4F3A}" name="S" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{4929AF3D-E527-44F8-83E4-6AE5FF5BA752}" name="Categorie" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{160D8024-BF24-4D71-A879-3001AEF28DB0}" name="Scop" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{68958FAA-582A-40BC-88E4-DFEFCD085D7D}" name="Given" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{58D080F2-3A38-4170-A080-888A61E6472D}" name="When" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{D820C683-EACB-473E-8174-BDFBE5643443}" name="Then" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{FE5DB5B8-32DD-4A39-8CE0-9093E1EA1F43}" name="Other" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3003,12 +3439,1266 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED31B81-665B-464C-9D97-28A7755B1692}">
+  <dimension ref="A1:G64"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="88.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CFEC01A-D47A-4916-AE5F-6864DC5658AC}">
+  <dimension ref="A1:G64"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="88.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7FA840-B515-494B-9270-DA5C4EDAADFC}">
   <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,15 +4804,21 @@
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>175</v>
+      </c>
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -4956,6 +6652,773 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C348F80-7090-4D4C-8D93-4F2C631A8533}">
+  <dimension ref="A1:I64"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" style="10" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14" style="3" customWidth="1"/>
+    <col min="7" max="8" width="42.140625" customWidth="1"/>
+    <col min="9" max="9" width="87.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+    </row>
+    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A89F87F-8119-49DC-8C57-CF2AF058D374}">
   <dimension ref="A1:G123"/>
   <sheetViews>
@@ -6045,12 +8508,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67517046-6F90-48A1-9B4E-378B133164D8}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6364,51 +8827,55 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="20"/>
+        <v>171</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="20"/>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -6417,99 +8884,103 @@
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>64</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E25" s="20"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>11</v>
-      </c>
-      <c r="B26" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
       <c r="C26" s="1" t="s">
-        <v>130</v>
+        <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>132</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E26" s="20"/>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>12</v>
-      </c>
-      <c r="B27" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3</v>
+      </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="20"/>
+        <v>131</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>132</v>
+      </c>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="20"/>
+        <v>66</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="11"/>
@@ -6523,7 +8994,7 @@
         <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="11"/>
@@ -6537,7 +9008,7 @@
         <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="11"/>
@@ -6551,35 +9022,35 @@
         <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="11"/>
@@ -6593,7 +9064,7 @@
         <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="11"/>
@@ -6607,7 +9078,7 @@
         <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="11"/>
@@ -6621,7 +9092,7 @@
         <v>16</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="11"/>
@@ -6635,7 +9106,7 @@
         <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="11"/>
@@ -6649,35 +9120,35 @@
         <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="11"/>
@@ -6691,7 +9162,7 @@
         <v>55</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="11"/>
@@ -6705,7 +9176,7 @@
         <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="11"/>
@@ -6719,7 +9190,7 @@
         <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="11"/>
@@ -6733,7 +9204,7 @@
         <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="11"/>
@@ -6747,7 +9218,7 @@
         <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="11"/>
@@ -6761,7 +9232,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="11"/>
@@ -6775,7 +9246,7 @@
         <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="11"/>
@@ -6789,7 +9260,7 @@
         <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="11"/>
@@ -6803,11 +9274,9 @@
         <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>49</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E51" s="20"/>
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6819,11 +9288,9 @@
         <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E52" s="20" t="s">
-        <v>50</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E52" s="20"/>
       <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6835,10 +9302,10 @@
         <v>55</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F53" s="11"/>
     </row>
@@ -6851,10 +9318,10 @@
         <v>55</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F54" s="11"/>
     </row>
@@ -6867,35 +9334,41 @@
         <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55" s="11"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>35</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F56" s="11"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>35</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="20"/>
-      <c r="F55" s="11"/>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>36</v>
-      </c>
-      <c r="C56" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="11"/>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>36</v>
-      </c>
-      <c r="C57" t="s">
-        <v>81</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E57" s="3"/>
+      <c r="E57" s="20"/>
       <c r="F57" s="11"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6906,7 +9379,7 @@
         <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="11"/>
@@ -6919,7 +9392,7 @@
         <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="11"/>
@@ -6932,7 +9405,7 @@
         <v>81</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="11"/>
@@ -6941,28 +9414,26 @@
       <c r="A61">
         <v>36</v>
       </c>
-      <c r="B61" s="1"/>
       <c r="C61" t="s">
         <v>81</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E61" s="20"/>
+        <v>51</v>
+      </c>
+      <c r="E61" s="3"/>
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>36</v>
       </c>
-      <c r="B62" s="1"/>
       <c r="C62" t="s">
         <v>81</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E62" s="20"/>
+        <v>53</v>
+      </c>
+      <c r="E62" s="3"/>
       <c r="F62" s="11"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6974,7 +9445,7 @@
         <v>81</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="11"/>
@@ -6988,7 +9459,7 @@
         <v>81</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="11"/>
@@ -7002,7 +9473,7 @@
         <v>81</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="11"/>
@@ -7016,7 +9487,7 @@
         <v>81</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="11"/>
@@ -7030,7 +9501,7 @@
         <v>81</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="11"/>
@@ -7044,7 +9515,7 @@
         <v>81</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="11"/>
@@ -7058,7 +9529,7 @@
         <v>81</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="11"/>
@@ -7072,7 +9543,7 @@
         <v>81</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="11"/>
@@ -7086,7 +9557,7 @@
         <v>81</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="11"/>
@@ -7100,7 +9571,7 @@
         <v>81</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="11"/>
@@ -7109,41 +9580,41 @@
       <c r="A73">
         <v>36</v>
       </c>
+      <c r="B73" s="1"/>
       <c r="C73" t="s">
         <v>81</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E73" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="E73" s="20"/>
       <c r="F73" s="11"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>37</v>
+      <c r="A74">
+        <v>36</v>
       </c>
       <c r="B74" s="1"/>
-      <c r="C74" s="1" t="s">
-        <v>83</v>
+      <c r="C74" t="s">
+        <v>81</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E74" s="20"/>
       <c r="F74" s="11"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>37</v>
-      </c>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1" t="s">
-        <v>83</v>
+      <c r="A75">
+        <v>36</v>
+      </c>
+      <c r="C75" t="s">
+        <v>81</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E75" s="20"/>
+        <v>80</v>
+      </c>
+      <c r="E75" s="3"/>
       <c r="F75" s="11"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -7155,7 +9626,7 @@
         <v>83</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="E76" s="20"/>
       <c r="F76" s="11"/>
@@ -7169,7 +9640,7 @@
         <v>83</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="11"/>
@@ -7183,7 +9654,7 @@
         <v>83</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="11"/>
@@ -7197,7 +9668,7 @@
         <v>83</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="11"/>
@@ -7211,7 +9682,7 @@
         <v>83</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="11"/>
@@ -7225,7 +9696,7 @@
         <v>83</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="11"/>
@@ -7239,7 +9710,7 @@
         <v>83</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="11"/>
@@ -7253,7 +9724,7 @@
         <v>83</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="11"/>
@@ -7267,7 +9738,7 @@
         <v>83</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="11"/>
@@ -7281,7 +9752,7 @@
         <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="11"/>
@@ -7295,7 +9766,7 @@
         <v>83</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="11"/>
@@ -7309,7 +9780,7 @@
         <v>83</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="11"/>
@@ -7323,7 +9794,7 @@
         <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="11"/>
@@ -7337,7 +9808,7 @@
         <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E89" s="20"/>
       <c r="F89" s="11"/>
@@ -7351,7 +9822,7 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="11"/>
@@ -7365,40 +9836,40 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E91" s="20"/>
       <c r="F91" s="11"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="E92" s="20"/>
       <c r="F92" s="11"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E93" s="20"/>
       <c r="F93" s="11"/>
     </row>
-    <row r="94" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>41</v>
       </c>
@@ -7407,7 +9878,7 @@
         <v>13</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E94" s="20"/>
       <c r="F94" s="11"/>
@@ -7421,39 +9892,39 @@
         <v>13</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E95" s="20" t="s">
-        <v>91</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E95" s="20"/>
       <c r="F95" s="11"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E96" s="20"/>
       <c r="F96" s="11"/>
     </row>
-    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E97" s="20"/>
+        <v>90</v>
+      </c>
+      <c r="E97" s="20" t="s">
+        <v>91</v>
+      </c>
       <c r="F97" s="11"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -7465,7 +9936,7 @@
         <v>55</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E98" s="20"/>
       <c r="F98" s="11"/>
@@ -7479,35 +9950,35 @@
         <v>55</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E99" s="20"/>
       <c r="F99" s="11"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>43</v>
+      <c r="A100" s="1">
+        <v>42</v>
       </c>
       <c r="B100" s="1"/>
-      <c r="C100" t="s">
-        <v>81</v>
+      <c r="C100" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E100" s="20"/>
       <c r="F100" s="11"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>43</v>
+      <c r="A101" s="1">
+        <v>42</v>
       </c>
       <c r="B101" s="1"/>
-      <c r="C101" t="s">
-        <v>81</v>
+      <c r="C101" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E101" s="20"/>
       <c r="F101" s="11"/>
@@ -7521,7 +9992,7 @@
         <v>81</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E102" s="20"/>
       <c r="F102" s="11"/>
@@ -7535,35 +10006,35 @@
         <v>81</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E103" s="20"/>
       <c r="F103" s="11"/>
     </row>
     <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>44</v>
+      <c r="A104">
+        <v>43</v>
       </c>
       <c r="B104" s="1"/>
-      <c r="C104" s="1" t="s">
-        <v>83</v>
+      <c r="C104" t="s">
+        <v>81</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E104" s="20"/>
       <c r="F104" s="11"/>
     </row>
     <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>44</v>
+      <c r="A105">
+        <v>43</v>
       </c>
       <c r="B105" s="1"/>
-      <c r="C105" s="1" t="s">
-        <v>83</v>
+      <c r="C105" t="s">
+        <v>81</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="11"/>
@@ -7577,7 +10048,7 @@
         <v>83</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="11"/>
@@ -7591,41 +10062,53 @@
         <v>83</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="11"/>
     </row>
     <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
+      <c r="A108" s="1">
+        <v>44</v>
+      </c>
       <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
+      <c r="C108" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="E108" s="20"/>
       <c r="F108" s="11"/>
     </row>
     <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E109" s="3"/>
+      <c r="A109" s="1">
+        <v>44</v>
+      </c>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E109" s="20"/>
       <c r="F109" s="11"/>
     </row>
     <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E110" s="3"/>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="20"/>
       <c r="F110" s="11"/>
     </row>
     <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="20"/>
+      <c r="E111" s="3"/>
       <c r="F111" s="11"/>
     </row>
     <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="20"/>
+      <c r="E112" s="3"/>
       <c r="F112" s="11"/>
     </row>
     <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -7779,6 +10262,22 @@
       <c r="D131" s="1"/>
       <c r="E131" s="20"/>
       <c r="F131" s="11"/>
+    </row>
+    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="20"/>
+      <c r="F132" s="11"/>
+    </row>
+    <row r="133" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="20"/>
+      <c r="F133" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7790,7 +10289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85EC9C-25A0-450D-AE0A-75CD9BA1329C}">
   <dimension ref="A1:G64"/>
   <sheetViews>
@@ -8420,12 +10919,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE23E348-29D0-4FF8-A4A5-A0998E1F2F1A}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8685,21 +11184,29 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="6"/>
+      <c r="D19" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="6"/>
+      <c r="D20" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>166</v>
+      </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
@@ -8707,8 +11214,12 @@
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
@@ -9108,7 +11619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1D129C-EF4C-42C0-8BBF-F86B855B079C}">
   <dimension ref="A1:I64"/>
   <sheetViews>
@@ -9866,626 +12377,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED31B81-665B-464C-9D97-28A7755B1692}">
-  <dimension ref="A1:G64"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="62.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="88.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Note	Add user to userlist Note	Delete user from Userlist
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81C74410-4492-4847-9472-8A818646A474}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0DE7EB5-FAE7-4A04-97B4-C61B9A0B6ED8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="183">
   <si>
     <t>N</t>
   </si>
@@ -726,6 +726,12 @@
   </si>
   <si>
     <t>checkIfIsAndOrLiked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete note form user </t>
+  </si>
+  <si>
+    <t>without createing noteuser repositori and service</t>
   </si>
 </sst>
 </file>
@@ -2571,7 +2577,6 @@
       <filters blank="1">
         <filter val="0"/>
         <filter val="1"/>
-        <filter val="2"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8513,7 +8518,7 @@
   <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8825,12 +8830,12 @@
       <c r="E20" s="1"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>13</v>
@@ -8843,12 +8848,12 @@
       </c>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2</v>
       </c>
       <c r="B22" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -8889,7 +8894,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -8905,7 +8910,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>9</v>
       </c>
@@ -8921,7 +8926,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>10</v>
       </c>
@@ -10923,8 +10928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE23E348-29D0-4FF8-A4A5-A0998E1F2F1A}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11227,8 +11232,12 @@
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="6"/>
+      <c r="D22" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>

</xml_diff>

<commit_message>
Note	Update Repository User	getUserList
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A47C989E-92D9-4811-999E-27B25E738DF6}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC0C8B44-1DD7-4D64-A9FA-24DE38BF85D8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="192">
   <si>
     <t>N</t>
   </si>
@@ -743,10 +743,26 @@
     <t>FDTO</t>
   </si>
   <si>
-    <t>modific pentru Remainder</t>
-  </si>
-  <si>
     <t>Update Repository</t>
+  </si>
+  <si>
+    <t>Get by Remainder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Every user has a list of users that with witch can share information
+ * To have access to other users information it has to request the conses
+ * You can have access only for the notes where you are included in the user list
+ * Cam be seen the users that are not in your user list? yes but you cannot see there content only if you are included by them int user list of there content</t>
+  </si>
+  <si>
+    <t>Add user in user List of the user
+When add a user to a note you can select form user list or ad a new user in the userlist and then select it</t>
+  </si>
+  <si>
+    <t>getUserList</t>
+  </si>
+  <si>
+    <t>modific pentru Remainder si user tag</t>
   </si>
 </sst>
 </file>
@@ -2457,10 +2473,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
@@ -2590,8 +2602,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F135" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="A1:F135" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F137" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:F137" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
     <filterColumn colId="1">
       <filters blank="1">
         <filter val="0"/>
@@ -2599,8 +2611,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F135">
-    <sortCondition ref="A1:A135"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F137">
+    <sortCondition ref="A1:A137"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="52"/>
@@ -4845,12 +4857,14 @@
       </c>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -8542,10 +8556,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67517046-6F90-48A1-9B4E-378B133164D8}">
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8579,7 +8593,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -8593,82 +8607,84 @@
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>185</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>186</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E5" s="20"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -8680,7 +8696,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11"/>
@@ -8694,7 +8710,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11"/>
@@ -8708,7 +8724,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="11"/>
@@ -8722,11 +8738,9 @@
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -8738,10 +8752,10 @@
         <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F12" s="11"/>
     </row>
@@ -8754,9 +8768,11 @@
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -8768,7 +8784,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="11"/>
@@ -8782,37 +8798,35 @@
         <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="11"/>
@@ -8826,11 +8840,9 @@
         <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>164</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E18" s="20"/>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -8842,10 +8854,10 @@
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F19" s="11"/>
     </row>
@@ -8858,9 +8870,11 @@
         <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="20"/>
+        <v>171</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -8872,7 +8886,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="11"/>
@@ -8886,7 +8900,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="11"/>
@@ -8897,21 +8911,21 @@
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1">
-        <v>4</v>
-      </c>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>56</v>
@@ -8928,7 +8942,7 @@
         <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="11"/>
@@ -8942,7 +8956,7 @@
         <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="11"/>
@@ -8956,9 +8970,9 @@
         <v>69</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="E27" s="20"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -8967,12 +8981,12 @@
         <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -8981,56 +8995,52 @@
         <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>49</v>
+        <v>147</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>11</v>
-      </c>
-      <c r="B30" s="1"/>
+    <row r="30" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1">
+        <v>4</v>
+      </c>
       <c r="C30" s="1" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>132</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>12</v>
-      </c>
-      <c r="B31" s="1"/>
+    <row r="31" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1">
+        <v>4</v>
+      </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>67</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="11"/>
@@ -9044,7 +9054,7 @@
         <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="11"/>
@@ -9058,7 +9068,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="11"/>
@@ -9072,35 +9082,39 @@
         <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>32</v>
-      </c>
-      <c r="B36" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
       <c r="C36" s="1" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="20"/>
+        <v>190</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>189</v>
+      </c>
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="11"/>
@@ -9114,7 +9128,7 @@
         <v>16</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="11"/>
@@ -9128,7 +9142,7 @@
         <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="11"/>
@@ -9142,7 +9156,7 @@
         <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="11"/>
@@ -9156,7 +9170,7 @@
         <v>16</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="11"/>
@@ -9170,7 +9184,7 @@
         <v>16</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="11"/>
@@ -9184,23 +9198,23 @@
         <v>16</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="E44" s="1"/>
       <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9961,7 +9975,7 @@
       <c r="E98" s="20"/>
       <c r="F98" s="11"/>
     </row>
-    <row r="99" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>41</v>
       </c>
@@ -9991,7 +10005,7 @@
       <c r="E100" s="20"/>
       <c r="F100" s="11"/>
     </row>
-    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>42</v>
       </c>
@@ -10147,34 +10161,46 @@
     </row>
     <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="20"/>
+      <c r="B112" s="1">
+        <v>4</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E112" s="1"/>
       <c r="F112" s="11"/>
     </row>
     <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E113" s="3"/>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1">
+        <v>3</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E113" s="20"/>
       <c r="F113" s="11"/>
     </row>
     <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E114" s="3"/>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="20"/>
       <c r="F114" s="11"/>
     </row>
     <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="20"/>
+      <c r="E115" s="3"/>
       <c r="F115" s="11"/>
     </row>
     <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="20"/>
+      <c r="E116" s="3"/>
       <c r="F116" s="11"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10328,6 +10354,22 @@
       <c r="D135" s="1"/>
       <c r="E135" s="20"/>
       <c r="F135" s="11"/>
+    </row>
+    <row r="136" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="20"/>
+      <c r="F136" s="11"/>
+    </row>
+    <row r="137" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="20"/>
+      <c r="F137" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- [x] getUserListByTagId - [x] getTopicListByTagId - [x] add created date to tag - [x] postTag - [x] getTagByTagId - [x] getAllTags
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9ED86DC-9456-40C6-9256-66BB94477F56}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9991A99-092C-4958-88FA-766E5E276732}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="1140" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="194">
   <si>
     <t>N</t>
   </si>
@@ -763,6 +763,14 @@
   </si>
   <si>
     <t>modific pentru Remainder si user tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`- If FDTO is defined I receive: spring.main.allow-circular-references
+  * I used in  NoteService is TagService
+  * </t>
+  </si>
+  <si>
+    <t>Not use FDTO</t>
   </si>
 </sst>
 </file>
@@ -2473,10 +2481,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
@@ -2988,8 +2992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2998,7 +3002,7 @@
     <col min="2" max="2" width="24.7109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65" style="16" customWidth="1"/>
-    <col min="5" max="5" width="162.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="61" style="10" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
@@ -3071,12 +3075,18 @@
       </c>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
+      <c r="B6" s="13" t="s">
+        <v>185</v>
+      </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
@@ -8562,8 +8572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67517046-6F90-48A1-9B4E-378B133164D8}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8625,12 +8635,12 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -8661,34 +8671,32 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>132</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E6" s="20"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>67</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E7" s="20"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -8823,14 +8831,14 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="11"/>
@@ -8925,14 +8933,14 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="11"/>
@@ -9037,56 +9045,60 @@
     </row>
     <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>32</v>
-      </c>
-      <c r="B32" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3</v>
+      </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="20"/>
+        <v>190</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>189</v>
+      </c>
       <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="11"/>
@@ -9095,18 +9107,14 @@
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="1">
-        <v>3</v>
-      </c>
+      <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>189</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E36" s="20"/>
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9118,7 +9126,7 @@
         <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="11"/>
@@ -9132,7 +9140,7 @@
         <v>16</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="11"/>
@@ -9146,63 +9154,63 @@
         <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="E40" s="1"/>
       <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="11"/>
@@ -9216,9 +9224,9 @@
         <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="E44" s="20"/>
       <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9230,7 +9238,7 @@
         <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="11"/>
@@ -9244,7 +9252,7 @@
         <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="11"/>
@@ -9258,7 +9266,7 @@
         <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="11"/>
@@ -9272,7 +9280,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="11"/>
@@ -9286,7 +9294,7 @@
         <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="11"/>
@@ -9300,7 +9308,7 @@
         <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="11"/>
@@ -9314,9 +9322,11 @@
         <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E51" s="20"/>
+        <v>50</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9328,9 +9338,11 @@
         <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="20"/>
+        <v>62</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9342,9 +9354,11 @@
         <v>55</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E53" s="20"/>
+        <v>78</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9356,9 +9370,11 @@
         <v>55</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E54" s="20"/>
+        <v>79</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="F54" s="11"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9370,73 +9386,61 @@
         <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>49</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E55" s="20"/>
       <c r="F55" s="11"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>35</v>
-      </c>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1" t="s">
-        <v>55</v>
+      <c r="A56">
+        <v>36</v>
+      </c>
+      <c r="C56" t="s">
+        <v>81</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>50</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E56" s="3"/>
       <c r="F56" s="11"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>35</v>
-      </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1" t="s">
-        <v>55</v>
+      <c r="A57">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>81</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>62</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E57" s="3"/>
       <c r="F57" s="11"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>35</v>
-      </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1" t="s">
-        <v>55</v>
+      <c r="A58">
+        <v>36</v>
+      </c>
+      <c r="C58" t="s">
+        <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>63</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E58" s="3"/>
       <c r="F58" s="11"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>35</v>
-      </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1" t="s">
-        <v>55</v>
+      <c r="A59">
+        <v>36</v>
+      </c>
+      <c r="C59" t="s">
+        <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E59" s="20"/>
+        <v>51</v>
+      </c>
+      <c r="E59" s="3"/>
       <c r="F59" s="11"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9447,7 +9451,7 @@
         <v>81</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="11"/>
@@ -9456,52 +9460,56 @@
       <c r="A61">
         <v>36</v>
       </c>
+      <c r="B61" s="1"/>
       <c r="C61" t="s">
         <v>81</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E61" s="3"/>
+        <v>59</v>
+      </c>
+      <c r="E61" s="20"/>
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>36</v>
       </c>
+      <c r="B62" s="1"/>
       <c r="C62" t="s">
         <v>81</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="E62" s="20"/>
       <c r="F62" s="11"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>36</v>
       </c>
+      <c r="B63" s="1"/>
       <c r="C63" t="s">
         <v>81</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E63" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="E63" s="20"/>
       <c r="F63" s="11"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>36</v>
       </c>
+      <c r="B64" s="1"/>
       <c r="C64" t="s">
         <v>81</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E64" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="E64" s="20"/>
       <c r="F64" s="11"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9513,7 +9521,7 @@
         <v>81</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="11"/>
@@ -9527,7 +9535,7 @@
         <v>81</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="11"/>
@@ -9541,7 +9549,7 @@
         <v>81</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="11"/>
@@ -9555,7 +9563,7 @@
         <v>81</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="11"/>
@@ -9569,7 +9577,7 @@
         <v>81</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="11"/>
@@ -9583,7 +9591,7 @@
         <v>81</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="11"/>
@@ -9597,7 +9605,7 @@
         <v>81</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="11"/>
@@ -9611,7 +9619,7 @@
         <v>81</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="11"/>
@@ -9620,69 +9628,69 @@
       <c r="A73">
         <v>36</v>
       </c>
-      <c r="B73" s="1"/>
       <c r="C73" t="s">
         <v>81</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E73" s="20"/>
+        <v>80</v>
+      </c>
+      <c r="E73" s="3"/>
       <c r="F73" s="11"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>36</v>
+      <c r="A74" s="1">
+        <v>37</v>
       </c>
       <c r="B74" s="1"/>
-      <c r="C74" t="s">
-        <v>81</v>
+      <c r="C74" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E74" s="20"/>
       <c r="F74" s="11"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>36</v>
+      <c r="A75" s="1">
+        <v>37</v>
       </c>
       <c r="B75" s="1"/>
-      <c r="C75" t="s">
-        <v>81</v>
+      <c r="C75" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E75" s="20"/>
       <c r="F75" s="11"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>36</v>
+      <c r="A76" s="1">
+        <v>37</v>
       </c>
       <c r="B76" s="1"/>
-      <c r="C76" t="s">
-        <v>81</v>
+      <c r="C76" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E76" s="20"/>
       <c r="F76" s="11"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>36</v>
-      </c>
-      <c r="C77" t="s">
-        <v>81</v>
+      <c r="A77" s="1">
+        <v>37</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E77" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="E77" s="20"/>
       <c r="F77" s="11"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9694,7 +9702,7 @@
         <v>83</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="11"/>
@@ -9708,7 +9716,7 @@
         <v>83</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="11"/>
@@ -9722,7 +9730,7 @@
         <v>83</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="11"/>
@@ -9736,7 +9744,7 @@
         <v>83</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="11"/>
@@ -9750,7 +9758,7 @@
         <v>83</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="11"/>
@@ -9764,7 +9772,7 @@
         <v>83</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="11"/>
@@ -9778,7 +9786,7 @@
         <v>83</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="11"/>
@@ -9792,7 +9800,7 @@
         <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="11"/>
@@ -9806,7 +9814,7 @@
         <v>83</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="11"/>
@@ -9820,7 +9828,7 @@
         <v>83</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="11"/>
@@ -9834,7 +9842,7 @@
         <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="11"/>
@@ -9848,7 +9856,7 @@
         <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="E89" s="20"/>
       <c r="F89" s="11"/>
@@ -9862,7 +9870,7 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="11"/>
@@ -9876,72 +9884,78 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E91" s="20"/>
       <c r="F91" s="11"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E92" s="20"/>
+        <v>131</v>
+      </c>
+      <c r="E92" s="20" t="s">
+        <v>132</v>
+      </c>
       <c r="F92" s="11"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E93" s="20"/>
+        <v>66</v>
+      </c>
+      <c r="E93" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F93" s="11"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E94" s="20"/>
       <c r="F94" s="11"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E95" s="20"/>
       <c r="F95" s="11"/>
     </row>
-    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>41</v>
       </c>
-      <c r="B96" s="1"/>
+      <c r="B96" s="1">
+        <v>4</v>
+      </c>
       <c r="C96" s="1" t="s">
         <v>13</v>
       </c>
@@ -9951,11 +9965,13 @@
       <c r="E96" s="20"/>
       <c r="F96" s="11"/>
     </row>
-    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>41</v>
       </c>
-      <c r="B97" s="1"/>
+      <c r="B97" s="1">
+        <v>4</v>
+      </c>
       <c r="C97" s="1" t="s">
         <v>13</v>
       </c>
@@ -9974,25 +9990,25 @@
         <v>13</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E98" s="20"/>
+        <v>90</v>
+      </c>
+      <c r="E98" s="20" t="s">
+        <v>91</v>
+      </c>
       <c r="F98" s="11"/>
     </row>
     <row r="99" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E99" s="20" t="s">
-        <v>91</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="E99" s="20"/>
       <c r="F99" s="11"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10004,7 +10020,7 @@
         <v>55</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E100" s="20"/>
       <c r="F100" s="11"/>
@@ -10018,7 +10034,7 @@
         <v>55</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E101" s="20"/>
       <c r="F101" s="11"/>
@@ -10032,21 +10048,21 @@
         <v>55</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E102" s="20"/>
       <c r="F102" s="11"/>
     </row>
     <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>42</v>
+      <c r="A103">
+        <v>43</v>
       </c>
       <c r="B103" s="1"/>
-      <c r="C103" s="1" t="s">
-        <v>55</v>
+      <c r="C103" t="s">
+        <v>81</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E103" s="20"/>
       <c r="F103" s="11"/>
@@ -10060,7 +10076,7 @@
         <v>81</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E104" s="20"/>
       <c r="F104" s="11"/>
@@ -10074,7 +10090,7 @@
         <v>81</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="11"/>
@@ -10088,21 +10104,21 @@
         <v>81</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="11"/>
     </row>
     <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>43</v>
+      <c r="A107" s="1">
+        <v>44</v>
       </c>
       <c r="B107" s="1"/>
-      <c r="C107" t="s">
-        <v>81</v>
+      <c r="C107" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="11"/>
@@ -10116,7 +10132,7 @@
         <v>83</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="11"/>
@@ -10130,7 +10146,7 @@
         <v>83</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="11"/>
@@ -10144,21 +10160,21 @@
         <v>83</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="11"/>
     </row>
     <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>44</v>
-      </c>
-      <c r="B111" s="1"/>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1">
+        <v>4</v>
+      </c>
       <c r="C111" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="E111" s="20"/>
       <c r="F111" s="11"/>

</xml_diff>

<commit_message>
- [x] getTagListByTopic - [x] getTagListByUser - [x] putUserToTag
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9991A99-092C-4958-88FA-766E5E276732}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E771EAA6-FCF9-4273-B04F-8FA6923B4BC8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="194">
   <si>
     <t>N</t>
   </si>
@@ -2481,6 +2481,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
@@ -2610,8 +2614,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F137" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="A1:F137" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{87FE02E0-FFDF-4944-A73E-E45CFAB31766}" name="Table13" displayName="Table13" ref="A1:F138" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:F138" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
     <filterColumn colId="1">
       <filters blank="1">
         <filter val="0"/>
@@ -2619,8 +2623,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F137">
-    <sortCondition ref="A1:A137"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F138">
+    <sortCondition ref="A1:A138"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="52"/>
@@ -2992,7 +2996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -8570,10 +8574,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67517046-6F90-48A1-9B4E-378B133164D8}">
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8689,7 +8693,9 @@
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>68</v>
       </c>
@@ -9043,36 +9049,36 @@
       <c r="E31" s="1"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>34</v>
-      </c>
-      <c r="B32" s="1">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>189</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>34</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1">
+        <v>3</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" s="20"/>
+        <v>190</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>189</v>
+      </c>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9084,7 +9090,7 @@
         <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="11"/>
@@ -9098,7 +9104,7 @@
         <v>16</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="11"/>
@@ -9112,7 +9118,7 @@
         <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="11"/>
@@ -9126,7 +9132,7 @@
         <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="11"/>
@@ -9140,7 +9146,7 @@
         <v>16</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="11"/>
@@ -9154,23 +9160,23 @@
         <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="E40" s="20"/>
       <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9182,9 +9188,9 @@
         <v>55</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E41" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="E41" s="1"/>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9196,7 +9202,7 @@
         <v>55</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="11"/>
@@ -9210,7 +9216,7 @@
         <v>55</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="11"/>
@@ -9224,7 +9230,7 @@
         <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="11"/>
@@ -9238,7 +9244,7 @@
         <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="11"/>
@@ -9252,7 +9258,7 @@
         <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="11"/>
@@ -9266,7 +9272,7 @@
         <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="11"/>
@@ -9280,7 +9286,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="11"/>
@@ -9294,7 +9300,7 @@
         <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="11"/>
@@ -9308,7 +9314,7 @@
         <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="11"/>
@@ -9322,11 +9328,9 @@
         <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>49</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E51" s="20"/>
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9338,10 +9342,10 @@
         <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F52" s="11"/>
     </row>
@@ -9354,10 +9358,10 @@
         <v>55</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F53" s="11"/>
     </row>
@@ -9370,10 +9374,10 @@
         <v>55</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F54" s="11"/>
     </row>
@@ -9386,22 +9390,25 @@
         <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F55" s="11"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>35</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="20"/>
-      <c r="F55" s="11"/>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>36</v>
-      </c>
-      <c r="C56" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E56" s="3"/>
+      <c r="E56" s="20"/>
       <c r="F56" s="11"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9412,7 +9419,7 @@
         <v>81</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="11"/>
@@ -9425,7 +9432,7 @@
         <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="11"/>
@@ -9438,7 +9445,7 @@
         <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="11"/>
@@ -9451,7 +9458,7 @@
         <v>81</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="11"/>
@@ -9460,14 +9467,13 @@
       <c r="A61">
         <v>36</v>
       </c>
-      <c r="B61" s="1"/>
       <c r="C61" t="s">
         <v>81</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E61" s="20"/>
+        <v>53</v>
+      </c>
+      <c r="E61" s="3"/>
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9479,7 +9485,7 @@
         <v>81</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="11"/>
@@ -9493,7 +9499,7 @@
         <v>81</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="11"/>
@@ -9507,7 +9513,7 @@
         <v>81</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="11"/>
@@ -9521,7 +9527,7 @@
         <v>81</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="11"/>
@@ -9535,7 +9541,7 @@
         <v>81</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="11"/>
@@ -9549,7 +9555,7 @@
         <v>81</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="11"/>
@@ -9563,7 +9569,7 @@
         <v>81</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="11"/>
@@ -9577,7 +9583,7 @@
         <v>81</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="11"/>
@@ -9591,7 +9597,7 @@
         <v>81</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="11"/>
@@ -9605,7 +9611,7 @@
         <v>81</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="11"/>
@@ -9619,7 +9625,7 @@
         <v>81</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="11"/>
@@ -9628,27 +9634,27 @@
       <c r="A73">
         <v>36</v>
       </c>
+      <c r="B73" s="1"/>
       <c r="C73" t="s">
         <v>81</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" s="20"/>
+      <c r="F73" s="11"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>36</v>
+      </c>
+      <c r="C74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="11"/>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>37</v>
-      </c>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E74" s="20"/>
+      <c r="E74" s="3"/>
       <c r="F74" s="11"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9660,7 +9666,7 @@
         <v>83</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E75" s="20"/>
       <c r="F75" s="11"/>
@@ -9674,7 +9680,7 @@
         <v>83</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E76" s="20"/>
       <c r="F76" s="11"/>
@@ -9688,7 +9694,7 @@
         <v>83</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="11"/>
@@ -9702,7 +9708,7 @@
         <v>83</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="11"/>
@@ -9716,7 +9722,7 @@
         <v>83</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="11"/>
@@ -9730,7 +9736,7 @@
         <v>83</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="11"/>
@@ -9744,7 +9750,7 @@
         <v>83</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="11"/>
@@ -9758,7 +9764,7 @@
         <v>83</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="11"/>
@@ -9772,7 +9778,7 @@
         <v>83</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="11"/>
@@ -9786,7 +9792,7 @@
         <v>83</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="11"/>
@@ -9800,7 +9806,7 @@
         <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="11"/>
@@ -9814,7 +9820,7 @@
         <v>83</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="11"/>
@@ -9828,7 +9834,7 @@
         <v>83</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="11"/>
@@ -9842,7 +9848,7 @@
         <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="11"/>
@@ -9856,7 +9862,7 @@
         <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E89" s="20"/>
       <c r="F89" s="11"/>
@@ -9870,7 +9876,7 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="11"/>
@@ -9884,40 +9890,38 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="E91" s="20"/>
       <c r="F91" s="11"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E92" s="20" t="s">
-        <v>132</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E92" s="20"/>
       <c r="F92" s="11"/>
     </row>
-    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>40</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="E93" s="20" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="F93" s="11"/>
     </row>
@@ -9927,40 +9931,40 @@
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E94" s="20"/>
+        <v>66</v>
+      </c>
+      <c r="E94" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F94" s="11"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E95" s="20"/>
       <c r="F95" s="11"/>
     </row>
-    <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>41</v>
       </c>
-      <c r="B96" s="1">
-        <v>4</v>
-      </c>
+      <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E96" s="20"/>
       <c r="F96" s="11"/>
@@ -9976,39 +9980,41 @@
         <v>13</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E97" s="20"/>
       <c r="F97" s="11"/>
     </row>
-    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>41</v>
       </c>
-      <c r="B98" s="1"/>
+      <c r="B98" s="1">
+        <v>4</v>
+      </c>
       <c r="C98" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E98" s="20" t="s">
-        <v>91</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E98" s="20"/>
       <c r="F98" s="11"/>
     </row>
     <row r="99" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E99" s="20"/>
+        <v>90</v>
+      </c>
+      <c r="E99" s="20" t="s">
+        <v>91</v>
+      </c>
       <c r="F99" s="11"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10020,7 +10026,7 @@
         <v>55</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E100" s="20"/>
       <c r="F100" s="11"/>
@@ -10034,7 +10040,7 @@
         <v>55</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E101" s="20"/>
       <c r="F101" s="11"/>
@@ -10048,21 +10054,21 @@
         <v>55</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E102" s="20"/>
       <c r="F102" s="11"/>
     </row>
     <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>43</v>
+      <c r="A103" s="1">
+        <v>42</v>
       </c>
       <c r="B103" s="1"/>
-      <c r="C103" t="s">
-        <v>81</v>
+      <c r="C103" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E103" s="20"/>
       <c r="F103" s="11"/>
@@ -10076,7 +10082,7 @@
         <v>81</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E104" s="20"/>
       <c r="F104" s="11"/>
@@ -10090,7 +10096,7 @@
         <v>81</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="11"/>
@@ -10104,21 +10110,21 @@
         <v>81</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="11"/>
     </row>
     <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>44</v>
+      <c r="A107">
+        <v>43</v>
       </c>
       <c r="B107" s="1"/>
-      <c r="C107" s="1" t="s">
-        <v>83</v>
+      <c r="C107" t="s">
+        <v>81</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="11"/>
@@ -10132,7 +10138,7 @@
         <v>83</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="11"/>
@@ -10146,7 +10152,7 @@
         <v>83</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="11"/>
@@ -10160,63 +10166,73 @@
         <v>83</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="11"/>
     </row>
     <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1">
-        <v>4</v>
-      </c>
+      <c r="A111" s="1">
+        <v>44</v>
+      </c>
+      <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="E111" s="20"/>
       <c r="F111" s="11"/>
     </row>
-    <row r="112" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1">
         <v>4</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E112" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="E112" s="20"/>
       <c r="F112" s="11"/>
     </row>
-    <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E113" s="20"/>
+        <v>186</v>
+      </c>
+      <c r="E113" s="1"/>
       <c r="F113" s="11"/>
     </row>
     <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
+      <c r="B114" s="1">
+        <v>3</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="E114" s="20"/>
       <c r="F114" s="11"/>
     </row>
     <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E115" s="3"/>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="20"/>
       <c r="F115" s="11"/>
     </row>
     <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10224,11 +10240,7 @@
       <c r="F116" s="11"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="20"/>
+      <c r="E117" s="3"/>
       <c r="F117" s="11"/>
     </row>
     <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10390,6 +10402,14 @@
       <c r="D137" s="1"/>
       <c r="E137" s="20"/>
       <c r="F137" s="11"/>
+    </row>
+    <row r="138" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="20"/>
+      <c r="F138" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- [x] getUserById - [x] getUserList - [x] putUserEmail - [x] putUserName
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E771EAA6-FCF9-4273-B04F-8FA6923B4BC8}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A53E222-1464-4422-AF64-817BF8CD4CCC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -2619,12 +2619,11 @@
     <filterColumn colId="1">
       <filters blank="1">
         <filter val="0"/>
-        <filter val="3"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F138">
-    <sortCondition ref="A1:A138"/>
+    <sortCondition ref="B1:B138"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A8648224-D12E-4BEE-803F-753FF2935F4B}" name="N" dataDxfId="52"/>
@@ -8577,7 +8576,7 @@
   <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8673,7 +8672,7 @@
       <c r="E5" s="20"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -8689,7 +8688,7 @@
       <c r="E6" s="20"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -8835,11 +8834,13 @@
       <c r="E16" s="20"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>68</v>
       </c>
@@ -8937,11 +8938,13 @@
       <c r="E23" s="20"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>68</v>
       </c>
@@ -9049,11 +9052,13 @@
       <c r="E31" s="1"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>5</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1">
+        <v>4</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>68</v>
       </c>
@@ -9063,83 +9068,81 @@
       <c r="E32" s="1"/>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>34</v>
-      </c>
+    <row r="33" spans="1:6" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
       <c r="B33" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>189</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E33" s="20"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="20"/>
+        <v>190</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>189</v>
+      </c>
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
@@ -9153,44 +9156,44 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E41" s="20"/>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9202,9 +9205,9 @@
         <v>55</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E42" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="E42" s="1"/>
       <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9216,7 +9219,7 @@
         <v>55</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="11"/>
@@ -9230,7 +9233,7 @@
         <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="11"/>
@@ -9244,7 +9247,7 @@
         <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="11"/>
@@ -9258,7 +9261,7 @@
         <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="11"/>
@@ -9272,7 +9275,7 @@
         <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="11"/>
@@ -9286,7 +9289,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="11"/>
@@ -9300,7 +9303,7 @@
         <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="11"/>
@@ -9314,7 +9317,7 @@
         <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="11"/>
@@ -9328,7 +9331,7 @@
         <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="11"/>
@@ -9342,11 +9345,9 @@
         <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="20" t="s">
-        <v>49</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E52" s="20"/>
       <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9358,10 +9359,10 @@
         <v>55</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F53" s="11"/>
     </row>
@@ -9374,10 +9375,10 @@
         <v>55</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F54" s="11"/>
     </row>
@@ -9390,10 +9391,10 @@
         <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F55" s="11"/>
     </row>
@@ -9406,22 +9407,25 @@
         <v>55</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F56" s="11"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>35</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E56" s="20"/>
-      <c r="F56" s="11"/>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>36</v>
-      </c>
-      <c r="C57" t="s">
-        <v>81</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E57" s="3"/>
+      <c r="E57" s="20"/>
       <c r="F57" s="11"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9432,7 +9436,7 @@
         <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="11"/>
@@ -9445,7 +9449,7 @@
         <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="11"/>
@@ -9458,7 +9462,7 @@
         <v>81</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="11"/>
@@ -9471,7 +9475,7 @@
         <v>81</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="11"/>
@@ -9480,14 +9484,13 @@
       <c r="A62">
         <v>36</v>
       </c>
-      <c r="B62" s="1"/>
       <c r="C62" t="s">
         <v>81</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E62" s="20"/>
+        <v>53</v>
+      </c>
+      <c r="E62" s="3"/>
       <c r="F62" s="11"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9499,7 +9502,7 @@
         <v>81</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="11"/>
@@ -9513,7 +9516,7 @@
         <v>81</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="11"/>
@@ -9527,7 +9530,7 @@
         <v>81</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="11"/>
@@ -9541,7 +9544,7 @@
         <v>81</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="11"/>
@@ -9555,7 +9558,7 @@
         <v>81</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="11"/>
@@ -9569,7 +9572,7 @@
         <v>81</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="11"/>
@@ -9583,7 +9586,7 @@
         <v>81</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="11"/>
@@ -9597,7 +9600,7 @@
         <v>81</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="11"/>
@@ -9611,7 +9614,7 @@
         <v>81</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="11"/>
@@ -9625,7 +9628,7 @@
         <v>81</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="11"/>
@@ -9639,7 +9642,7 @@
         <v>81</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E73" s="20"/>
       <c r="F73" s="11"/>
@@ -9648,27 +9651,27 @@
       <c r="A74">
         <v>36</v>
       </c>
+      <c r="B74" s="1"/>
       <c r="C74" t="s">
         <v>81</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E74" s="20"/>
+      <c r="F74" s="11"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>36</v>
+      </c>
+      <c r="C75" t="s">
+        <v>81</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="11"/>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>37</v>
-      </c>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E75" s="20"/>
+      <c r="E75" s="3"/>
       <c r="F75" s="11"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9680,7 +9683,7 @@
         <v>83</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E76" s="20"/>
       <c r="F76" s="11"/>
@@ -9694,7 +9697,7 @@
         <v>83</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="11"/>
@@ -9708,7 +9711,7 @@
         <v>83</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="11"/>
@@ -9722,7 +9725,7 @@
         <v>83</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="11"/>
@@ -9736,7 +9739,7 @@
         <v>83</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="11"/>
@@ -9750,7 +9753,7 @@
         <v>83</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="11"/>
@@ -9764,7 +9767,7 @@
         <v>83</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="11"/>
@@ -9778,7 +9781,7 @@
         <v>83</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="11"/>
@@ -9792,7 +9795,7 @@
         <v>83</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="11"/>
@@ -9806,7 +9809,7 @@
         <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="11"/>
@@ -9820,7 +9823,7 @@
         <v>83</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="11"/>
@@ -9834,7 +9837,7 @@
         <v>83</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="11"/>
@@ -9848,7 +9851,7 @@
         <v>83</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="11"/>
@@ -9862,7 +9865,7 @@
         <v>83</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E89" s="20"/>
       <c r="F89" s="11"/>
@@ -9876,7 +9879,7 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="11"/>
@@ -9890,7 +9893,7 @@
         <v>83</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E91" s="20"/>
       <c r="F91" s="11"/>
@@ -9904,25 +9907,23 @@
         <v>83</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="E92" s="20"/>
       <c r="F92" s="11"/>
     </row>
     <row r="93" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E93" s="20" t="s">
-        <v>132</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E93" s="20"/>
       <c r="F93" s="11"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9931,13 +9932,13 @@
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="E94" s="20" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="F94" s="11"/>
     </row>
@@ -9947,24 +9948,26 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E95" s="20"/>
+        <v>66</v>
+      </c>
+      <c r="E95" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="F95" s="11"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="E96" s="20"/>
       <c r="F96" s="11"/>
@@ -10010,25 +10013,25 @@
         <v>13</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E99" s="20" t="s">
-        <v>91</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E99" s="20"/>
       <c r="F99" s="11"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E100" s="20"/>
+        <v>90</v>
+      </c>
+      <c r="E100" s="20" t="s">
+        <v>91</v>
+      </c>
       <c r="F100" s="11"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10040,7 +10043,7 @@
         <v>55</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E101" s="20"/>
       <c r="F101" s="11"/>
@@ -10054,7 +10057,7 @@
         <v>55</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E102" s="20"/>
       <c r="F102" s="11"/>
@@ -10068,21 +10071,21 @@
         <v>55</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E103" s="20"/>
       <c r="F103" s="11"/>
     </row>
     <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>43</v>
+      <c r="A104" s="1">
+        <v>42</v>
       </c>
       <c r="B104" s="1"/>
-      <c r="C104" t="s">
-        <v>81</v>
+      <c r="C104" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E104" s="20"/>
       <c r="F104" s="11"/>
@@ -10096,7 +10099,7 @@
         <v>81</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="11"/>
@@ -10110,7 +10113,7 @@
         <v>81</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="11"/>
@@ -10124,21 +10127,21 @@
         <v>81</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="11"/>
     </row>
     <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <v>44</v>
+      <c r="A108">
+        <v>43</v>
       </c>
       <c r="B108" s="1"/>
-      <c r="C108" s="1" t="s">
-        <v>83</v>
+      <c r="C108" t="s">
+        <v>81</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="11"/>
@@ -10152,7 +10155,7 @@
         <v>83</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="11"/>
@@ -10166,7 +10169,7 @@
         <v>83</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="11"/>
@@ -10180,12 +10183,12 @@
         <v>83</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E111" s="20"/>
       <c r="F111" s="11"/>
     </row>
-    <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1">
         <v>4</v>
@@ -10214,15 +10217,15 @@
       <c r="F113" s="11"/>
     </row>
     <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1">
-        <v>3</v>
-      </c>
+      <c r="A114" s="1">
+        <v>44</v>
+      </c>
+      <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>187</v>
+        <v>90</v>
       </c>
       <c r="E114" s="20"/>
       <c r="F114" s="11"/>

</xml_diff>

<commit_message>
- [x] Add to all OneToMany the orphanRemoval and cascade - [x] postTopic
</commit_message>
<xml_diff>
--- a/FO.xlsx
+++ b/FO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1637275a1ccf8178/Java/FO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A4FA908-A9EE-414B-818F-3935B0D820E5}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{041D69F1-87AA-440F-942A-1A62FEA9BF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{965284BF-9B3A-4525-8B1B-123D1620FA28}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-8280" yWindow="735" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -2484,10 +2484,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A1:E62" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}"/>
@@ -2621,6 +2617,7 @@
   <autoFilter ref="A1:F138" xr:uid="{91D804A7-BE3A-4F9A-A8DC-F3737400C5AC}">
     <filterColumn colId="1">
       <filters blank="1">
+        <filter val="?"/>
         <filter val="0"/>
       </filters>
     </filterColumn>
@@ -8578,8 +8575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67517046-6F90-48A1-9B4E-378B133164D8}">
   <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9151,11 +9148,13 @@
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="1">
+        <v>4</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>16</v>
       </c>
@@ -9165,18 +9164,18 @@
       <c r="E38" s="20"/>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>3</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>194</v>
+        <v>5</v>
+      </c>
+      <c r="B39" s="1">
+        <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>187</v>
+        <v>61</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="11"/>
@@ -9199,14 +9198,16 @@
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>5</v>
-      </c>
-      <c r="B41" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="C41" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>61</v>
+        <v>187</v>
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="11"/>

</xml_diff>